<commit_message>
insert NXB, NCC, THELOAI, THETHUVIEN, DAUSACH, SACH-TG
</commit_message>
<xml_diff>
--- a/TTCSDL.xlsx
+++ b/TTCSDL.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Downloads\Ky2Nam3\Thuc tap Co so du lieu\TTCSDL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dinhv\OneDrive\Máy tính\TTCSDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="345" windowWidth="20940" windowHeight="9870" firstSheet="18" activeTab="19"/>
+    <workbookView xWindow="630" yWindow="345" windowWidth="20940" windowHeight="9870" tabRatio="896" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="TACGIA" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,10 @@
     <sheet name="PHIEUNHAP" sheetId="19" r:id="rId19"/>
     <sheet name="PHIEUXUAT" sheetId="20" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">NHANVIEN!$C$1:$C$20</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="232">
   <si>
     <t>MaTacGia</t>
   </si>
@@ -60,15 +63,9 @@
     <t xml:space="preserve">Minh Ngọc </t>
   </si>
   <si>
-    <t>82 Phố Lý Thái Tổ, Lý Thái Tổ, Hoàn Kiếm, Hà Nội</t>
-  </si>
-  <si>
     <t xml:space="preserve">Huỳnh Khải Vệ </t>
   </si>
   <si>
-    <t>123/5B Lê Lợi, Phường 6, Tuy Hòa,  Phú Yên</t>
-  </si>
-  <si>
     <t>MaKeSach</t>
   </si>
   <si>
@@ -204,266 +201,577 @@
     <t xml:space="preserve">Phạm Anh Thư </t>
   </si>
   <si>
+    <t>Nguyễn Nhật Ánh</t>
+  </si>
+  <si>
+    <t>Ki Ju Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiểu Thuyết </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kệ Sách A </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kệ Sách B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kệ Sách C </t>
+  </si>
+  <si>
+    <t>Kệ Sách D</t>
+  </si>
+  <si>
+    <t>Kệ Sách E</t>
+  </si>
+  <si>
+    <t>Truyện Ngắn - Tản Văn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chính Trị - Pháp Luật </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Văn Học Nghệ Thuật </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Khoa Học Công Nghệ </t>
+  </si>
+  <si>
+    <t>Kho 1A</t>
+  </si>
+  <si>
+    <t>Kho 1B</t>
+  </si>
+  <si>
+    <t>Kho 2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kho 2B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phòng 301 , Tầng 3, Tòa H2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phòng 302 , Tầng 3, Tòa H2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phòng 401 , Tầng 4, Tòa H2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phòng 402 , Tầng 4, Tòa H2 </t>
+  </si>
+  <si>
+    <t>Skybooks</t>
+  </si>
+  <si>
+    <t>Công ty cổ phần MTV Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NXB Trẻ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thiên Long </t>
+  </si>
+  <si>
+    <t>Số 50 đường 5, TTF 361 An Dương, Tây Hồ, Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">161B Lý Chính Thắng, Phường 7,Quận 3,Hồ Chí Minh.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhà Sách Trí Việt </t>
+  </si>
+  <si>
+    <t>234 Tây Sơn, Trung Liệt, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>Số 7/33 Ngõ 199 Hồ Tùng Mậu - Phường Cầu Diễn - Quận Nam Từ Liêm - Hà Nội</t>
+  </si>
+  <si>
+    <t>NXB Phụ Nữ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NXB Lao Động </t>
+  </si>
+  <si>
+    <t>NXB Trẻ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NXB Kim Đồng </t>
+  </si>
+  <si>
+    <t>62 Nguyễn Thị Minh Khai, Phường Đa Kao, Quận 1, TP.HCM</t>
+  </si>
+  <si>
+    <t>55 Quang Trung, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>39 Hàng Chuối, Q. Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Còn Hạn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mất Sách </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mất, hỏng tem mã vạch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rách bìa, bung bìa </t>
+  </si>
+  <si>
+    <t>Bẩn sách</t>
+  </si>
+  <si>
+    <t>Giữ sách quá hạn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Vũ hải Anh </t>
+  </si>
+  <si>
+    <t>KTPM16</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
+  </si>
+  <si>
+    <t>Phạm Đức Anh</t>
+  </si>
+  <si>
+    <t>Ninh Bình</t>
+  </si>
+  <si>
+    <t>Phạm Hoàng Anh</t>
+  </si>
+  <si>
+    <t>Hải Dương</t>
+  </si>
+  <si>
+    <t>Trần Đức Anh</t>
+  </si>
+  <si>
+    <t>Trần Tuấn Anh</t>
+  </si>
+  <si>
+    <t>Mình Về Hà Nội Để Thương Nhau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tiếc Rằng Mình Chẳng Đợi Được Nhau </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Có Một Cô Gái Thầm Yêu Anh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tôi Thấy Hoa Vàng Trên Cỏ Xanh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nhiệt Độ Ngôn Ngữ </t>
+  </si>
+  <si>
+    <t>Số 4, phố Tống Duy Tân, quận Hoàn Kiếm, thành phố Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đã mượn </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kho C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phòng 403,Tầng 4 ,Tòa H2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Thi Như Quỳnh </t>
+  </si>
+  <si>
+    <t>Quách Văn Thắng</t>
+  </si>
+  <si>
+    <t>Lê Đình Tú</t>
+  </si>
+  <si>
+    <t>Nguyễn Ánh Dương</t>
+  </si>
+  <si>
+    <t>Trần Cao Thanh Tùng</t>
+  </si>
+  <si>
+    <t>028 38 225 340</t>
+  </si>
+  <si>
+    <t>Số 6/86 Duy Tân, Cầu Giấy, Hà Nội; </t>
+  </si>
+  <si>
+    <t>81 Trần Hưng Đạo, Hà Nội</t>
+  </si>
+  <si>
+    <t>Số 65 Nguyễn Du, Hà Nội</t>
+  </si>
+  <si>
+    <t>Số 35 Trần Quốc Toản, Hoàn Kiếm, Hà Nội</t>
+  </si>
+  <si>
+    <t>Tầng 6, Tòa nhà Cục Tần số Vô tuyến điện, số 115 Trần Duy Hưng, Hà Nội </t>
+  </si>
+  <si>
+    <t>024 35772145</t>
+  </si>
+  <si>
+    <t>80B Trần Hưng Đạo, Hoàn Kiếm, Hà Nội</t>
+  </si>
+  <si>
+    <t>024 3942334</t>
+  </si>
+  <si>
+    <t>16 Hàng Chuối, Phạm Đình Hổ, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>Khu phố 6, P. Linh Trung, Q. Thủ Đức, TP. HCM</t>
+  </si>
+  <si>
+    <t>028 6681 7058</t>
+  </si>
+  <si>
+    <t>18, Nguyễn Trường Tộ, Trúc Bạch, Ba Đình, Hà Nội</t>
+  </si>
+  <si>
+    <t>Đại học Oxford</t>
+  </si>
+  <si>
+    <t>Đại học Cambridge</t>
+  </si>
+  <si>
+    <t>65, Tràng Thi, Hà Nội</t>
+  </si>
+  <si>
+    <t>NXB Tri Thức</t>
+  </si>
+  <si>
+    <t>23 Lý Nam Đế, Hoàn Kiếm, Hà Nội</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NXB QUÂN ĐỘI NHÂN DÂN </t>
+  </si>
+  <si>
+    <t>Tầng 1, Tòa nhà VUSTA, 53, Nguyễn Du, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>024 3945 4661</t>
+  </si>
+  <si>
+    <t>Sách Công Nghệ Thông Tin</t>
+  </si>
+  <si>
+    <t>Sách Giáo Khoa - Giáo Trình </t>
+  </si>
+  <si>
+    <t>Sách Học Ngoại Ngữ</t>
+  </si>
+  <si>
+    <t>Sách Kiến Thức Tổng Hợp</t>
+  </si>
+  <si>
+    <t>Sách Tham Khảo</t>
+  </si>
+  <si>
+    <t>Sách Thường Thức - Gia Đình</t>
+  </si>
+  <si>
+    <t>Sách Tâm lý - Giới tính</t>
+  </si>
+  <si>
+    <t>Sách Y Học</t>
+  </si>
+  <si>
+    <t>Sách kinh tế </t>
+  </si>
+  <si>
+    <t>Sách kỹ năng sống</t>
+  </si>
+  <si>
+    <t>Sách thiếu nhi</t>
+  </si>
+  <si>
+    <t>Sách Lịch sử</t>
+  </si>
+  <si>
+    <t>Sách Văn Hóa - Địa Lý - Du Lịch</t>
+  </si>
+  <si>
+    <t>Sách Tôn Giáo - Tâm Linh</t>
+  </si>
+  <si>
+    <t>175 Giảng Võ, Đống Đa, Hà Nội175 Giảng Võ, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t> 024 3971 4896</t>
+  </si>
+  <si>
+    <t>Cô Gái Đến Từ Hôm Qua</t>
+  </si>
+  <si>
+    <t>Mắt Biếc</t>
+  </si>
+  <si>
+    <t>Cho Tôi Xin Một Vé Đi Tuổi Thơ</t>
+  </si>
+  <si>
+    <t>Có Hai Con Mèo Ngồi Bên Cửa Sổ</t>
+  </si>
+  <si>
+    <t>Tôi Là Bêtô</t>
+  </si>
+  <si>
+    <t>Ngồi Khóc Trên Cây: Truyện Dài</t>
+  </si>
+  <si>
+    <t>John C. Maxwell</t>
+  </si>
+  <si>
+    <t> 15 Nguyên Tắc Vàng Về Phát Triển Bản Thân</t>
+  </si>
+  <si>
+    <t>NXB Hà Nội</t>
+  </si>
+  <si>
+    <t>NXB Tổng hợp thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>NXB chính trị quốc gia sự thật</t>
+  </si>
+  <si>
+    <t>NXB giáo dục</t>
+  </si>
+  <si>
+    <t>NXB Hội Nhà văn</t>
+  </si>
+  <si>
+    <t>NXB Tư pháp</t>
+  </si>
+  <si>
+    <t>NXB thông tin và truyền thông</t>
+  </si>
+  <si>
+    <t>NXB giao thông vận tải</t>
+  </si>
+  <si>
+    <t>NXB Đại học Quốc Gia Hà Nội</t>
+  </si>
+  <si>
+    <t>NXB Đại học Quốc gia Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>NXB Văn Học</t>
+  </si>
+  <si>
+    <t>NXB Đại học Oxford</t>
+  </si>
+  <si>
+    <t>NXB Đại học Cambridge</t>
+  </si>
+  <si>
+    <t>NXB Hồng Đức</t>
+  </si>
+  <si>
+    <t>NXB Thế giới</t>
+  </si>
+  <si>
+    <t>46 Trần Hưng Đạo, Hàng Bài, Hoàn Kiếm, Hà Nội </t>
+  </si>
+  <si>
+    <t>024 3825 3841</t>
+  </si>
+  <si>
+    <t>Trở Thành Người Ảnh Hưởng</t>
+  </si>
+  <si>
+    <t>Thái Độ 101 – Những Điều Nhà Lãnh Đạo Cần Biết</t>
+  </si>
+  <si>
+    <t>Mối Quan Hệ 101 – Những Điều Nhà Lãnh Đạo Cần Biết</t>
+  </si>
+  <si>
+    <t>Tiki Trading</t>
+  </si>
+  <si>
+    <t>Nhà sách Fahasa</t>
+  </si>
+  <si>
+    <t>Nhà sách Thanh Hà</t>
+  </si>
+  <si>
+    <t> ALPHA BOOKS</t>
+  </si>
+  <si>
+    <t> AZ VIỆT NAM</t>
+  </si>
+  <si>
+    <t>FIRST NEWS TRÍ VIỆT</t>
+  </si>
+  <si>
+    <t> Văn Hóa Văn Lang</t>
+  </si>
+  <si>
+    <t>TÂN VIỆT</t>
+  </si>
+  <si>
+    <t>PANDA BOOKS</t>
+  </si>
+  <si>
+    <t> SÁCH MINH LONG</t>
+  </si>
+  <si>
+    <t>Vinabook JSC</t>
+  </si>
+  <si>
+    <t>Nhà Sách Sao Mai</t>
+  </si>
+  <si>
+    <t>52 Út Tịch, phường 4, quận Tân Bình, thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>60 - 62 Lê Lợi, Quận 1, TP. HCM, Việt Nam</t>
+  </si>
+  <si>
+    <t>Thanh Hà Books NV5.36 khu đô thị Viglacera phường Tây Mỗ quận Nam Từ Liêm, Từ Liêm</t>
+  </si>
+  <si>
+    <t>0388 553 222</t>
+  </si>
+  <si>
+    <t>176 Thái Hà, Trung Liệt, Đống Đa, Hà Nội</t>
+  </si>
+  <si>
+    <t>Số 56 - Đường 5 - Khu tập thể F361 - phố An Dương - P. Yên Phụ - Q.Tây Hồ - HN</t>
+  </si>
+  <si>
+    <t>11H Nguyễn Thị Minh Khai, Phường Bến Nghé, Quận 1, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>06 Nguyễn Trung Trực, P.5, Q. Bình Thạnh, TP.HCM</t>
+  </si>
+  <si>
+    <t> 449 Bạch Mai - Hai Bà Trưng - Hà Nội</t>
+  </si>
+  <si>
+    <t>B8/20 Đầm Trấu, Hai Bà Trưng, Hà Nội., Bạch Đằng, Hai Bà Trưng, Hà Nội</t>
+  </si>
+  <si>
+    <t>024 3856 9432</t>
+  </si>
+  <si>
+    <t>số 17 Ngô Quyền – 34 Tràng Tiền, phường Tràng Tiền, quận Hoàn Kiếm, TP Hà Nội</t>
+  </si>
+  <si>
+    <t>Nhà Số 1, Lô A7, Khu Đô Thị Đầm Trấu, Phường Bạch Đằng, Quận Hai Bà Trưng, Thành Phố Hà Nội</t>
+  </si>
+  <si>
+    <t>024 6294 3819</t>
+  </si>
+  <si>
+    <t>71 Đông Hồ, phường 8, quận Tân Bình, Thành phố Hồ Chí Minh</t>
+  </si>
+  <si>
+    <t>44 Xô Viết Nghệ Tĩnh, Phường 19, Quận Bình Thạnh, TP. Hồ Chí Minh</t>
+  </si>
+  <si>
     <r>
-      <t>84 Võ Chí Công, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF555555"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
       <t> </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF333333"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>Quận Tây Hồ</t>
+      <t>093 232 99 59</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t> </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FF555555"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, Hà Nội</t>
-    </r>
-  </si>
-  <si>
-    <t>Bình Quế, Thăng Bình, Quảng Nam</t>
-  </si>
-  <si>
-    <t>Nguyễn Nhật Ánh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hàn Quốc </t>
-  </si>
-  <si>
-    <t>Ki Ju Lee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiểu Thuyết </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kệ Sách A </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kệ Sách B </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kệ Sách C </t>
-  </si>
-  <si>
-    <t>Kệ Sách D</t>
-  </si>
-  <si>
-    <t>Kệ Sách E</t>
-  </si>
-  <si>
-    <t>Truyện Ngắn - Tản Văn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chính Trị - Pháp Luật </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Văn Học Nghệ Thuật </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Khoa Học Công Nghệ </t>
-  </si>
-  <si>
-    <t>Kho 1A</t>
-  </si>
-  <si>
-    <t>Kho 1B</t>
-  </si>
-  <si>
-    <t>Kho 2A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kho 2B </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phòng 301 , Tầng 3, Tòa H2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phòng 302 , Tầng 3, Tòa H2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phòng 401 , Tầng 4, Tòa H2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phòng 402 , Tầng 4, Tòa H2 </t>
-  </si>
-  <si>
-    <t>Skybooks</t>
-  </si>
-  <si>
-    <t>Công ty cổ phần MTV Hà Nội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NXB Trẻ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thiên Long </t>
-  </si>
-  <si>
-    <t>Số 50 đường 5, TTF 361 An Dương, Tây Hồ, Hà Nội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Số nhà 38, ngách 88b, ngõ 49, phố Thúy Lĩnh, Phường Lĩnh Nam,  Hoàng Mai, Hà Nội
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">161B Lý Chính Thắng, Phường 7,Quận 3,Hồ Chí Minh.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nhà Sách Trí Việt </t>
-  </si>
-  <si>
-    <t>234 Tây Sơn, Trung Liệt, Đống Đa, Hà Nội</t>
-  </si>
-  <si>
-    <t>Số 7/33 Ngõ 199 Hồ Tùng Mậu - Phường Cầu Diễn - Quận Nam Từ Liêm - Hà Nội</t>
-  </si>
-  <si>
-    <t>NXB Phụ Nữ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NXB Lao Động </t>
-  </si>
-  <si>
-    <t>NXB Trẻ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NXB Kim Đồng </t>
-  </si>
-  <si>
-    <t>62 Nguyễn Thị Minh Khai, Phường Đa Kao, Quận 1, TP.HCM</t>
-  </si>
-  <si>
-    <t>55 Quang Trung, Hai Bà Trưng, Hà Nội</t>
-  </si>
-  <si>
-    <r>
-      <t>175 Giảng Võ, Đống Đa, Hà Nội</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>175 Giảng Võ, Đống Đa, Hà Nội</t>
+      <t>CTY CP MTV HÀ NỘI</t>
     </r>
   </si>
   <si>
-    <t>39 Hàng Chuối, Q. Hai Bà Trưng, Hà Nội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Còn Hạn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mất Sách </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mất, hỏng tem mã vạch </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rách bìa, bung bìa </t>
-  </si>
-  <si>
-    <t>Bẩn sách</t>
-  </si>
-  <si>
-    <t>Giữ sách quá hạn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Vũ hải Anh </t>
-  </si>
-  <si>
-    <t>KTPM16</t>
-  </si>
-  <si>
-    <t>Hà Nội</t>
-  </si>
-  <si>
-    <t>Phạm Đức Anh</t>
-  </si>
-  <si>
-    <t>Ninh Bình</t>
-  </si>
-  <si>
-    <t>Phạm Hoàng Anh</t>
-  </si>
-  <si>
-    <t>Hải Dương</t>
-  </si>
-  <si>
-    <t>Trần Đức Anh</t>
-  </si>
-  <si>
-    <t>Trần Tuấn Anh</t>
-  </si>
-  <si>
-    <t>Mình Về Hà Nội Để Thương Nhau</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiếc Rằng Mình Chẳng Đợi Được Nhau </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Có Một Cô Gái Thầm Yêu Anh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tôi Thấy Hoa Vàng Trên Cỏ Xanh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nhiệt Độ Ngôn Ngữ </t>
-  </si>
-  <si>
-    <t>Nhà Xuất Bản Hà Nội</t>
-  </si>
-  <si>
-    <t>Số 4, phố Tống Duy Tân, quận Hoàn Kiếm, thành phố Hà Nội</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Đã mượn </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kho C </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phòng 403,Tầng 4 ,Tòa H2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Thi Như Quỳnh </t>
-  </si>
-  <si>
-    <t>Quách Văn Thắng</t>
-  </si>
-  <si>
-    <t>Lê Đình Tú</t>
-  </si>
-  <si>
-    <t>Nguyễn Ánh Dương</t>
-  </si>
-  <si>
-    <t>Trần Cao Thanh Tùng</t>
+    <t>08 62 935 574</t>
+  </si>
+  <si>
+    <t>Nhà sách Thái Hà</t>
+  </si>
+  <si>
+    <t>119 C5 Tô Hiệu, Khu tập thể Nghĩa Tân, Cầu Giấy, Hà Nội</t>
+  </si>
+  <si>
+    <t>024 6281 3638</t>
+  </si>
+  <si>
+    <t> 02838242157 </t>
+  </si>
+  <si>
+    <t>028 35140632</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38, ngách 88b, ngõ 49, phố Thúy Lĩnh, Phường Lĩnh Nam,  Hoàng Mai, Hà Nội
+</t>
+  </si>
+  <si>
+    <t>Trương Anh Khoa</t>
+  </si>
+  <si>
+    <t>Đặng Quang Vũ</t>
+  </si>
+  <si>
+    <t>Nguyễn Bích Như</t>
+  </si>
+  <si>
+    <t>Vũ Kim Phượng</t>
+  </si>
+  <si>
+    <t>Nguyễn Phương Quyên</t>
+  </si>
+  <si>
+    <t>Phùng Ðức Bảo</t>
+  </si>
+  <si>
+    <t>Phạm Diệu Loan</t>
+  </si>
+  <si>
+    <t>Trần Ngọc Yến</t>
+  </si>
+  <si>
+    <t>Dương Thu Trang</t>
+  </si>
+  <si>
+    <t>Đoàn Bích Hằng</t>
+  </si>
+  <si>
+    <t>Võ Việt An</t>
+  </si>
+  <si>
+    <t>Nguyễn Khắc Duy</t>
+  </si>
+  <si>
+    <t>Phạm Phương Thảo</t>
+  </si>
+  <si>
+    <t>Hồ Ngọc Huệ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -474,35 +782,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF555555"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <color rgb="FF313131"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -522,23 +830,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -817,101 +1154,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView topLeftCell="BK1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>18576</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>288765456</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>18577</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>497645764</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>18578</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4">
-        <v>375646476</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>18579</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5">
-        <v>375768355</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>18580</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6">
-        <v>526756747</v>
-      </c>
-      <c r="D6" t="s">
-        <v>56</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>18580</v>
+      </c>
+      <c r="B7" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -922,96 +1230,223 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
+      <c r="A1" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="9">
         <v>90</v>
       </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="9">
         <v>551</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="9">
         <v>91</v>
       </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="9">
         <v>551</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="9">
         <v>92</v>
       </c>
-      <c r="B4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="9">
         <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="9">
         <v>93</v>
       </c>
-      <c r="B5" t="s">
-        <v>112</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="9">
         <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="9">
         <v>94</v>
       </c>
-      <c r="B6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" s="9">
         <v>555</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>95</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="9">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>96</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C8" s="9">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>97</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C9" s="9">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>98</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" s="9">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>99</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="9">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>100</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="9">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>101</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="9">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>102</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="9">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>103</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="C15" s="9">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>104</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="9">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1457,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1065,6 +1500,86 @@
         <v>94</v>
       </c>
       <c r="B6">
+        <v>18580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>95</v>
+      </c>
+      <c r="B7">
+        <v>18579</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>96</v>
+      </c>
+      <c r="B8">
+        <v>18579</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>97</v>
+      </c>
+      <c r="B9">
+        <v>18579</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>98</v>
+      </c>
+      <c r="B10">
+        <v>18579</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>99</v>
+      </c>
+      <c r="B11">
+        <v>18579</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>18579</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>18580</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>102</v>
+      </c>
+      <c r="B14">
+        <v>18580</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>103</v>
+      </c>
+      <c r="B15">
+        <v>18580</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>104</v>
+      </c>
+      <c r="B16">
         <v>18580</v>
       </c>
     </row>
@@ -1091,26 +1606,26 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>122</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="1">
         <v>43891</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>43904</v>
       </c>
       <c r="D2">
@@ -1121,10 +1636,10 @@
       <c r="A3">
         <v>123</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="1">
         <v>43894</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <v>43908</v>
       </c>
       <c r="D3">
@@ -1135,10 +1650,10 @@
       <c r="A4">
         <v>124</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="1">
         <v>43927</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1">
         <v>43934</v>
       </c>
       <c r="D4">
@@ -1149,10 +1664,10 @@
       <c r="A5">
         <v>125</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="1">
         <v>43892</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="1">
         <v>43899</v>
       </c>
       <c r="D5">
@@ -1163,10 +1678,10 @@
       <c r="A6">
         <v>126</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="1">
         <v>43891</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="1">
         <v>43900</v>
       </c>
       <c r="D6">
@@ -1195,20 +1710,20 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>321</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="1">
         <v>43904</v>
       </c>
       <c r="C2">
@@ -1219,7 +1734,7 @@
       <c r="A3">
         <v>322</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="1">
         <v>43908</v>
       </c>
       <c r="C3">
@@ -1230,7 +1745,7 @@
       <c r="A4">
         <v>323</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="1">
         <v>43934</v>
       </c>
       <c r="C4">
@@ -1241,7 +1756,7 @@
       <c r="A5">
         <v>324</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="1">
         <v>43899</v>
       </c>
       <c r="C5">
@@ -1252,7 +1767,7 @@
       <c r="A6">
         <v>325</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="1">
         <v>43900</v>
       </c>
       <c r="C6">
@@ -1286,28 +1801,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
       <c r="E1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1315,13 +1830,13 @@
         <v>10001000</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C2">
         <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E2">
         <v>90</v>
@@ -1341,13 +1856,13 @@
         <v>10001001</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C3">
         <v>250</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E3">
         <v>91</v>
@@ -1367,13 +1882,13 @@
         <v>10001002</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C4">
         <v>178</v>
       </c>
       <c r="D4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E4">
         <v>92</v>
@@ -1393,13 +1908,13 @@
         <v>10001003</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C5">
         <v>378</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E5">
         <v>93</v>
@@ -1419,13 +1934,13 @@
         <v>10001004</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C6">
         <v>232</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E6">
         <v>94</v>
@@ -1463,26 +1978,26 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>101</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="1">
         <v>43891</v>
       </c>
       <c r="C2">
@@ -1499,7 +2014,7 @@
       <c r="A3">
         <v>102</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="1">
         <v>43892</v>
       </c>
       <c r="C3">
@@ -1516,7 +2031,7 @@
       <c r="A4">
         <v>103</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="1">
         <v>43891</v>
       </c>
       <c r="C4">
@@ -1533,7 +2048,7 @@
       <c r="A5">
         <v>104</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="1">
         <v>43898</v>
       </c>
       <c r="C5">
@@ -1550,7 +2065,7 @@
       <c r="A6">
         <v>105</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="1">
         <v>43891</v>
       </c>
       <c r="C6">
@@ -1570,82 +2085,237 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
+      <c r="A1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="8">
         <v>2201</v>
       </c>
-      <c r="B2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" s="8">
         <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="8">
         <v>2202</v>
       </c>
-      <c r="B3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="8">
         <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="8">
         <v>2203</v>
       </c>
-      <c r="B4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="8">
         <v>331</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="8">
         <v>2204</v>
       </c>
-      <c r="B5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="8">
         <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="8">
         <v>2205</v>
       </c>
-      <c r="B6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="8">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>2206</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="C7" s="8">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>2207</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="8">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>2208</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="C9" s="8">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>2209</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C10" s="8">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>2210</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" s="8">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>2211</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="C12" s="8">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>2212</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="8">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>2213</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="C14" s="8">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>2214</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15" s="8">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>2215</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="C16" s="8">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>2216</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="C17" s="8">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>2217</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="C18" s="8">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>2218</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" s="8">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>2219</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="C20" s="8">
         <v>433</v>
       </c>
     </row>
@@ -1670,10 +2340,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1737,10 +2407,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1805,13 +2475,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1821,7 +2491,7 @@
       <c r="B2">
         <v>4441</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>43863</v>
       </c>
     </row>
@@ -1832,7 +2502,7 @@
       <c r="B3">
         <v>4442</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <v>43863</v>
       </c>
     </row>
@@ -1843,7 +2513,7 @@
       <c r="B4">
         <v>4443</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1">
         <v>43863</v>
       </c>
     </row>
@@ -1854,7 +2524,7 @@
       <c r="B5">
         <v>4444</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="1">
         <v>43863</v>
       </c>
     </row>
@@ -1865,7 +2535,7 @@
       <c r="B6">
         <v>4445</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="1">
         <v>43863</v>
       </c>
     </row>
@@ -1879,7 +2549,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,10 +2560,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1901,7 +2571,7 @@
         <v>1110</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1909,7 +2579,7 @@
         <v>1111</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1917,7 +2587,7 @@
         <v>1112</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1925,7 +2595,7 @@
         <v>1113</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1933,7 +2603,7 @@
         <v>1114</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1945,7 +2615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1959,13 +2629,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1975,7 +2645,7 @@
       <c r="B2">
         <v>1110</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="1">
         <v>43875</v>
       </c>
     </row>
@@ -1986,7 +2656,7 @@
       <c r="B3">
         <v>1111</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="1">
         <v>43875</v>
       </c>
     </row>
@@ -1997,7 +2667,7 @@
       <c r="B4">
         <v>1112</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="1">
         <v>43875</v>
       </c>
     </row>
@@ -2008,7 +2678,7 @@
       <c r="B5">
         <v>1113</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="1">
         <v>43875</v>
       </c>
     </row>
@@ -2019,7 +2689,7 @@
       <c r="B6">
         <v>1114</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="1">
         <v>43875</v>
       </c>
     </row>
@@ -2031,10 +2701,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="CJ1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2045,10 +2715,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2056,7 +2726,7 @@
         <v>1110</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2064,7 +2734,7 @@
         <v>1111</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2072,7 +2742,7 @@
         <v>1112</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2750,7 @@
         <v>1113</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2758,119 @@
         <v>1114</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1113</v>
+      </c>
+      <c r="B10" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1114</v>
+      </c>
+      <c r="B11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1113</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1114</v>
+      </c>
+      <c r="B16" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1110</v>
+      </c>
+      <c r="B17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1112</v>
+      </c>
+      <c r="B19" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1113</v>
+      </c>
+      <c r="B20" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -2101,7 +2883,7 @@
   <dimension ref="A7:C12"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A8" sqref="A8:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,13 +2895,13 @@
   <sheetData>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2127,10 +2909,10 @@
         <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2138,10 +2920,10 @@
         <v>222</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2149,10 +2931,10 @@
         <v>331</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2160,10 +2942,10 @@
         <v>332</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2171,10 +2953,10 @@
         <v>433</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2184,210 +2966,617 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="71.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24" style="9" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="71.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="12" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>4441</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="12">
+        <v>437172838</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>4442</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2436805252</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>4443</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2">
-        <v>437172838</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4442</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D4" s="12">
+        <v>2839316289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4444</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3">
-        <v>2436805252</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4443</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4">
-        <v>84.028393162889998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4444</v>
-      </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="D5" s="12">
         <v>983928269</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>4445</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6">
+      <c r="D6" s="12">
         <v>969318982</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>4446</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D7" s="13">
+        <v>19006035</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>4447</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D8" s="12">
+        <v>1900636467</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>4448</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>4449</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>4450</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D11" s="12">
+        <v>2432567333</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>4451</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D12" s="12">
+        <v>2838227979</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>4452</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>4453</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>4454</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D15" s="12">
+        <v>2439728108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>4455</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="12">
+        <v>43934063</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>4456</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>4457</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>4458</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>4459</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" display="https://www.google.com/search?sxsrf=ALeKk00b4RV78nzuTrxI0Qx6e4X8D1MW0w:1585321531520&amp;q=nh%C3%A0+cung+c%E1%BA%A5p+s%C3%A1ch&amp;npsic=0&amp;rflfq=1&amp;rlha=0&amp;rllag=20993706,105799133,3366&amp;tbm=lcl&amp;ved=2ahUKEwjpuPb19rroAhXaZt4KHdlHCtoQjGp6BAgLEDs&amp;tbs=lrf:!1m4!1u3!2m2!3m1!1e1!1m4!1u2!2m2!2m1!1e1!2m1!1e2!2m1!1e3!3sIAE,lf:1,lf_ui:10&amp;rldoc=1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="GJ1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="43.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="53.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>551</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="7">
         <v>2439710717</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="6">
         <v>552</v>
       </c>
-      <c r="B3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="7">
         <v>2438515380</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>553</v>
       </c>
-      <c r="B4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="7">
         <v>2838225340</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="6">
         <v>554</v>
       </c>
-      <c r="B5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="7">
         <v>2439434730</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="6">
         <v>555</v>
       </c>
-      <c r="B6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="7">
         <v>438252916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>556</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>557</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="7">
+        <v>28049221</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>558</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="7">
+        <v>2438220801</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>559</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2438222135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>560</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2462632078</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>561</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>562</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>563</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>564</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>565</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>566</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>567</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>568</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>569</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>570</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="7">
+        <v>2438455766</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>571</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2398,42 +3587,42 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>17150001</v>
       </c>
-      <c r="B2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="1">
         <v>44601</v>
       </c>
       <c r="D2">
@@ -2444,10 +3633,10 @@
       <c r="A3">
         <v>17150002</v>
       </c>
-      <c r="B3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="1">
         <v>44777</v>
       </c>
       <c r="D3">
@@ -2458,10 +3647,10 @@
       <c r="A4">
         <v>17150003</v>
       </c>
-      <c r="B4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="1">
         <v>45049</v>
       </c>
       <c r="D4">
@@ -2472,10 +3661,10 @@
       <c r="A5">
         <v>17150004</v>
       </c>
-      <c r="B5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="5">
+      <c r="B5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="1">
         <v>45272</v>
       </c>
       <c r="D5">
@@ -2486,13 +3675,521 @@
       <c r="A6">
         <v>17150005</v>
       </c>
-      <c r="B6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C6" s="5">
+      <c r="B6" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="1">
         <v>44878</v>
       </c>
       <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>17150006</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44601</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>17150007</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44777</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>17150008</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="1">
+        <v>45049</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>17150009</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45272</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>17150010</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44878</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>17150011</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44601</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>17150012</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" s="1">
+        <v>44777</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>17150013</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="1">
+        <v>45049</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>17150014</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45272</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>17150015</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" s="1">
+        <v>44878</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17150016</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="1">
+        <v>44601</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17150017</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45272</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17150018</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44878</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17150019</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44601</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17150020</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45272</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17150021</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C22" s="1">
+        <v>44878</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>17150022</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="1">
+        <v>44601</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>17150023</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="1">
+        <f ca="1">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
+        <v>45236</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>17150024</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" ref="C25:C41" ca="1" si="0">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
+        <v>44595</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>17150025</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="1">
+        <f ca="1">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
+        <v>44517</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>17150026</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44963</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>17150027</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44535</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>17150028</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44625</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>17150029</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44235</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>17150030</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44500</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>17150031</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45063</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>17150032</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45063</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>17150033</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45124</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>17150034</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44784</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>17150035</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44572</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>17150036</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44395</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>17150037</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44506</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>17150038</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45095</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>17150039</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45164</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>17150040</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45209</v>
+      </c>
+      <c r="D41">
         <v>1</v>
       </c>
     </row>
@@ -2519,16 +4216,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2536,7 +4233,7 @@
         <v>7878</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D2">
         <v>17150023</v>
@@ -2547,7 +4244,7 @@
         <v>7879</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D3">
         <v>16150020</v>
@@ -2558,7 +4255,7 @@
         <v>7890</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="D4">
         <v>18150465</v>
@@ -2569,7 +4266,7 @@
         <v>7891</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="D5">
         <v>18150673</v>
@@ -2580,7 +4277,7 @@
         <v>7892</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D6">
         <v>15150511</v>
@@ -2596,7 +4293,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2612,16 +4309,16 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" t="s">
-        <v>32</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -2630,7 +4327,7 @@
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2638,16 +4335,16 @@
         <v>1111110</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" s="5">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1">
         <v>36263</v>
       </c>
       <c r="E2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F2">
         <v>367069763</v>
@@ -2661,16 +4358,16 @@
         <v>1111111</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="5">
+        <v>94</v>
+      </c>
+      <c r="D3" s="1">
         <v>36356</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F3">
         <v>364974368</v>
@@ -2684,16 +4381,16 @@
         <v>1111112</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="5">
+        <v>94</v>
+      </c>
+      <c r="D4" s="1">
         <v>36258</v>
       </c>
       <c r="E4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="F4">
         <v>966166821</v>
@@ -2707,16 +4404,16 @@
         <v>1111113</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
-      </c>
-      <c r="D5" s="5">
+        <v>94</v>
+      </c>
+      <c r="D5" s="1">
         <v>36186</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F5">
         <v>971889405</v>
@@ -2730,16 +4427,16 @@
         <v>1111114</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D6" s="5">
+        <v>94</v>
+      </c>
+      <c r="D6" s="1">
         <v>36350</v>
       </c>
       <c r="E6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="F6">
         <v>397114855</v>

</xml_diff>

<commit_message>
Insert DOCGIA, THETHUVIEN, NHANVIEN
</commit_message>
<xml_diff>
--- a/TTCSDL.xlsx
+++ b/TTCSDL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="345" windowWidth="20940" windowHeight="9870" tabRatio="896" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="630" yWindow="345" windowWidth="20940" windowHeight="9870" tabRatio="896" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="TACGIA" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="371">
   <si>
     <t>MaTacGia</t>
   </si>
@@ -766,6 +766,423 @@
   </si>
   <si>
     <t>Hồ Ngọc Huệ</t>
+  </si>
+  <si>
+    <t>CAO HẢI ANH</t>
+  </si>
+  <si>
+    <t>ĐỖ ĐỨC ANH</t>
+  </si>
+  <si>
+    <t>MAI QUANG VIỆT ANH</t>
+  </si>
+  <si>
+    <t>PHẠM ĐỨC ANH</t>
+  </si>
+  <si>
+    <t>TẠ NGỌC ANH</t>
+  </si>
+  <si>
+    <t>TRẦN TIẾN ANH</t>
+  </si>
+  <si>
+    <t>NGUYỄN ĐĂNG NHẬT ANH</t>
+  </si>
+  <si>
+    <t>NGUYỄN THẾ ANH</t>
+  </si>
+  <si>
+    <t>PHẠM THẾ ANH</t>
+  </si>
+  <si>
+    <t>TRỊNH XUÂN ANH</t>
+  </si>
+  <si>
+    <t>PHẠM HOÀNG ANH</t>
+  </si>
+  <si>
+    <t>TRẦN THÁI BẢO</t>
+  </si>
+  <si>
+    <t>NGUYỄN ĐỨC BẮC</t>
+  </si>
+  <si>
+    <t>HOÀNG THỊ CHUNG</t>
+  </si>
+  <si>
+    <t>ĐẬU THÀNH VĂN CHƯƠNG</t>
+  </si>
+  <si>
+    <t>VŨ THÀNH CÔNG</t>
+  </si>
+  <si>
+    <t>Ngô Mạnh Cường</t>
+  </si>
+  <si>
+    <t>NGUYỄN THÁI CƯỜNG</t>
+  </si>
+  <si>
+    <t>PHONG ĐỨC DUY</t>
+  </si>
+  <si>
+    <t>VŨ XUÂN DUY</t>
+  </si>
+  <si>
+    <t>TĂNG VIỆT DŨNG</t>
+  </si>
+  <si>
+    <t>NGUYỄN VĂN DŨNG</t>
+  </si>
+  <si>
+    <t>BÙI TUẤN DƯƠNG</t>
+  </si>
+  <si>
+    <t>PHẠM HẢI DƯƠNG</t>
+  </si>
+  <si>
+    <t>NGUYỄN TIẾN ĐẠT</t>
+  </si>
+  <si>
+    <t>ĐẶNG QUANG ĐẠT</t>
+  </si>
+  <si>
+    <t>LÊ TIẾN ĐẠT</t>
+  </si>
+  <si>
+    <t>NGUYỄN THÀNH ĐẠT</t>
+  </si>
+  <si>
+    <t>LÊ XUÂN ĐÔNG</t>
+  </si>
+  <si>
+    <t>NGUYỄN MINH ĐỨC</t>
+  </si>
+  <si>
+    <t>ĐỖ THỊ HƯƠNG GIANG</t>
+  </si>
+  <si>
+    <t>NGUYỄN THỊ THU HÀ</t>
+  </si>
+  <si>
+    <t>NGUYỄN QUÍ HẢI</t>
+  </si>
+  <si>
+    <t>ĐẶNG THỊ HIỀN</t>
+  </si>
+  <si>
+    <t>ĐINH ĐỨC HIẾU</t>
+  </si>
+  <si>
+    <t>VŨ VĂN HIẾU</t>
+  </si>
+  <si>
+    <t>NGUYỄN VĂN HIỆU</t>
+  </si>
+  <si>
+    <t>LỖ TRUNG HIẾU</t>
+  </si>
+  <si>
+    <t>NGUYỄN MINH HIẾU</t>
+  </si>
+  <si>
+    <t>ĐINH THỊ HOÀI</t>
+  </si>
+  <si>
+    <t>LÊ VIỆT HOÀNG</t>
+  </si>
+  <si>
+    <t>Lê Minh Hoàng</t>
+  </si>
+  <si>
+    <t>Mai Nhật Hoàng</t>
+  </si>
+  <si>
+    <t>NGUYỄN HOÀNG</t>
+  </si>
+  <si>
+    <t>THÁI VIỆT HOÀNG</t>
+  </si>
+  <si>
+    <t>DƯƠNG NGỌC HUY</t>
+  </si>
+  <si>
+    <t>NGUYỄN QUANG HUY</t>
+  </si>
+  <si>
+    <t>Ngô Đình Huy</t>
+  </si>
+  <si>
+    <t>Phan Ngọc Huy</t>
+  </si>
+  <si>
+    <t>ĐỒNG VĂN HÙNG</t>
+  </si>
+  <si>
+    <t>NGUYỄN TUẤN HÙNG</t>
+  </si>
+  <si>
+    <t>NGUYỄN QUANG HƯNG</t>
+  </si>
+  <si>
+    <t>NGUYỄN VĂN KHÁ</t>
+  </si>
+  <si>
+    <t>CAO DUY KHANG</t>
+  </si>
+  <si>
+    <t>NGUYỄN QUỐC KHÁNH</t>
+  </si>
+  <si>
+    <t>ĐẶNG QUỐC KHÁNH</t>
+  </si>
+  <si>
+    <t>VŨ VIỆT LÂM</t>
+  </si>
+  <si>
+    <t>ĐẶNG THỊ LINH</t>
+  </si>
+  <si>
+    <t>HOÀNG NGỌC LINH</t>
+  </si>
+  <si>
+    <t>BÙI CÔNG LONG</t>
+  </si>
+  <si>
+    <t>NGUYỄN HOÀNG LONG</t>
+  </si>
+  <si>
+    <t>NGUYỄN HỮU LỘC</t>
+  </si>
+  <si>
+    <t>ĐINH VĂN LỰC</t>
+  </si>
+  <si>
+    <t>NGUYỄN HÙNG MẠNH</t>
+  </si>
+  <si>
+    <t>Thái Đức Mạnh</t>
+  </si>
+  <si>
+    <t>NGUYỄN THỊ MÂY</t>
+  </si>
+  <si>
+    <t>HOÀNG QUANG MINH</t>
+  </si>
+  <si>
+    <t>TRỊNH ĐỨC NHẬT MINH</t>
+  </si>
+  <si>
+    <t>BÙI THỊ TRÀ MY</t>
+  </si>
+  <si>
+    <t>Đoàn Quang Nam</t>
+  </si>
+  <si>
+    <t>LÊ PHƯƠNG NAM</t>
+  </si>
+  <si>
+    <t>TRƯƠNG TUẤN NGHĨA</t>
+  </si>
+  <si>
+    <t>PHÙNG THỊ NGỌC</t>
+  </si>
+  <si>
+    <t>ĐINH CÔNG PHONG</t>
+  </si>
+  <si>
+    <t>NGUYỄN VĂN PHONG</t>
+  </si>
+  <si>
+    <t>VŨ ĐÌNH QUANG</t>
+  </si>
+  <si>
+    <t>NGUYỄN MINH QUÂN</t>
+  </si>
+  <si>
+    <t>NGUYỄN ĐÌNH NHƯ QUỲNH</t>
+  </si>
+  <si>
+    <t>NGUYỄN XUÂN SƠN</t>
+  </si>
+  <si>
+    <t>TDH17</t>
+  </si>
+  <si>
+    <t>DTVT17</t>
+  </si>
+  <si>
+    <t>DKCN</t>
+  </si>
+  <si>
+    <t>CNTT16A</t>
+  </si>
+  <si>
+    <t>CNM15</t>
+  </si>
+  <si>
+    <t>HTTTQL15</t>
+  </si>
+  <si>
+    <t>GAM&amp;MP14</t>
+  </si>
+  <si>
+    <t>CDT17</t>
+  </si>
+  <si>
+    <t>TDH 16</t>
+  </si>
+  <si>
+    <t>CNTT16B</t>
+  </si>
+  <si>
+    <t>DPT13</t>
+  </si>
+  <si>
+    <t>DDT14C</t>
+  </si>
+  <si>
+    <t>CNPM15</t>
+  </si>
+  <si>
+    <t>CNDL15</t>
+  </si>
+  <si>
+    <t>CDT15B</t>
+  </si>
+  <si>
+    <t>DDT14B</t>
+  </si>
+  <si>
+    <t>DTVT16B</t>
+  </si>
+  <si>
+    <t>ĐTYS14</t>
+  </si>
+  <si>
+    <t>CN_CNDL15</t>
+  </si>
+  <si>
+    <t>0977632345 </t>
+  </si>
+  <si>
+    <t>0946186898 </t>
+  </si>
+  <si>
+    <t>DTVT14</t>
+  </si>
+  <si>
+    <t>Quảng Ninh</t>
+  </si>
+  <si>
+    <t>Kon Tum</t>
+  </si>
+  <si>
+    <t>Bắc Ninh</t>
+  </si>
+  <si>
+    <t>Quảng Bình</t>
+  </si>
+  <si>
+    <t>Thừa Thiên Huế</t>
+  </si>
+  <si>
+    <t>Vĩnh Long</t>
+  </si>
+  <si>
+    <t>Ninh Thuận</t>
+  </si>
+  <si>
+    <t>Cà Mau</t>
+  </si>
+  <si>
+    <t>Khánh Hòa</t>
+  </si>
+  <si>
+    <t>Đồng Nai</t>
+  </si>
+  <si>
+    <t>Vĩnh Phúc</t>
+  </si>
+  <si>
+    <t>Phú Yên</t>
+  </si>
+  <si>
+    <t>Trà Vinh</t>
+  </si>
+  <si>
+    <t>Thái Nguyên</t>
+  </si>
+  <si>
+    <t>Thanh Hóa</t>
+  </si>
+  <si>
+    <t>Hậu Giang</t>
+  </si>
+  <si>
+    <t>Hòa Bình</t>
+  </si>
+  <si>
+    <t>Quảng Trị</t>
+  </si>
+  <si>
+    <t>Bạc Liêu</t>
+  </si>
+  <si>
+    <t>Đắk Nông</t>
+  </si>
+  <si>
+    <t>Bắc Giang</t>
+  </si>
+  <si>
+    <t>Long An</t>
+  </si>
+  <si>
+    <t>Kiên Giang</t>
+  </si>
+  <si>
+    <t>Bình Dương</t>
+  </si>
+  <si>
+    <t>Cao Bằng</t>
+  </si>
+  <si>
+    <t>Tiền Giang</t>
+  </si>
+  <si>
+    <t>Lạng Sơn</t>
+  </si>
+  <si>
+    <t>Cần Thơ</t>
+  </si>
+  <si>
+    <t>Hà Nam</t>
+  </si>
+  <si>
+    <t>Đồng Tháp</t>
+  </si>
+  <si>
+    <t>Nam Định</t>
+  </si>
+  <si>
+    <t>Nghệ An</t>
+  </si>
+  <si>
+    <t>Sóc Trăng</t>
+  </si>
+  <si>
+    <t>Bến Tre</t>
+  </si>
+  <si>
+    <t>Bình Thuận</t>
+  </si>
+  <si>
+    <t>Lai Châu</t>
+  </si>
+  <si>
+    <t>Bắc Kạn</t>
+  </si>
+  <si>
+    <t>Đắk Lắk</t>
   </si>
 </sst>
 </file>
@@ -1232,7 +1649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -2883,7 +3300,7 @@
   <dimension ref="A7:C12"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A12"/>
+      <selection activeCell="A7" sqref="A7:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3587,10 +4004,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection sqref="A1:D84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3673,7 +4090,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>17150005</v>
+        <v>18150230</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>87</v>
@@ -3687,7 +4104,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>17150006</v>
+        <v>18150169</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>87</v>
@@ -3701,7 +4118,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>17150007</v>
+        <v>18150232</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>87</v>
@@ -3715,7 +4132,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>17150008</v>
+        <v>18150172</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>87</v>
@@ -3729,7 +4146,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>17150009</v>
+        <v>18150173</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>87</v>
@@ -3743,7 +4160,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>17150010</v>
+        <v>18150174</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>87</v>
@@ -3757,7 +4174,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>17150011</v>
+        <v>18150233</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>87</v>
@@ -3771,7 +4188,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>17150012</v>
+        <v>18150171</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>87</v>
@@ -3785,7 +4202,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>17150013</v>
+        <v>18150234</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>87</v>
@@ -3799,7 +4216,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>17150014</v>
+        <v>18150238</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>87</v>
@@ -3813,7 +4230,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>17150015</v>
+        <v>17150003</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>87</v>
@@ -3827,7 +4244,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>17150016</v>
+        <v>17150085</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>87</v>
@@ -3841,7 +4258,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17150017</v>
+        <v>18150175</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>87</v>
@@ -3855,7 +4272,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>17150018</v>
+        <v>16150084</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>87</v>
@@ -3869,7 +4286,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>17150019</v>
+        <v>18150179</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>87</v>
@@ -3883,7 +4300,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>17150020</v>
+        <v>16150229</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>87</v>
@@ -3897,7 +4314,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>17150021</v>
+        <v>15150015</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>87</v>
@@ -3911,7 +4328,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>17150022</v>
+        <v>18150123</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>87</v>
@@ -3925,14 +4342,14 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>17150023</v>
+        <v>18150187</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="1">
         <f ca="1">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
-        <v>45236</v>
+        <v>44685</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3940,14 +4357,14 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>17150024</v>
+        <v>18150188</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ref="C25:C41" ca="1" si="0">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
-        <v>44595</v>
+        <f t="shared" ref="C25:C84" ca="1" si="0">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
+        <v>44615</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -3955,14 +4372,14 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>17150025</v>
+        <v>18150185</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C26" s="1">
         <f ca="1">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
-        <v>44517</v>
+        <v>45189</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -3970,14 +4387,14 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>17150026</v>
+        <v>17151004</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44963</v>
+        <v>45181</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -3985,14 +4402,14 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>17150027</v>
+        <v>18150248</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44535</v>
+        <v>44820</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -4000,14 +4417,14 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>17150028</v>
+        <v>18150249</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44625</v>
+        <v>44784</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -4015,14 +4432,14 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>17150029</v>
+        <v>18150181</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44235</v>
+        <v>44694</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -4030,14 +4447,14 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>17150030</v>
+        <v>17150008</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44500</v>
+        <v>45240</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -4045,14 +4462,14 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>17150031</v>
+        <v>17150424</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45063</v>
+        <v>44332</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -4060,14 +4477,14 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>17150032</v>
+        <v>17150010</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45063</v>
+        <v>44740</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -4075,14 +4492,14 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>17150033</v>
+        <v>18150183</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45124</v>
+        <v>45112</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -4090,14 +4507,14 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>17150034</v>
+        <v>18150246</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44784</v>
+        <v>44454</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -4105,14 +4522,14 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>17150035</v>
+        <v>18150189</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44572</v>
+        <v>44358</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -4120,14 +4537,14 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>17150036</v>
+        <v>17150020</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44395</v>
+        <v>45218</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -4135,14 +4552,14 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>17150037</v>
+        <v>18150190</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44506</v>
+        <v>45230</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -4150,14 +4567,14 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>17150038</v>
+        <v>16150100</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45095</v>
+        <v>44632</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -4165,14 +4582,14 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>17150039</v>
+        <v>18150255</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45164</v>
+        <v>45178</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -4180,17 +4597,705 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>17150040</v>
+        <v>18150256</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>87</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45209</v>
+        <v>44680</v>
       </c>
       <c r="D41">
         <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>18150257</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44527</v>
+      </c>
+      <c r="D42">
+        <f ca="1">RANDBETWEEN(0, 4)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>17151003</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44693</v>
+      </c>
+      <c r="D43">
+        <f t="shared" ref="D43:D84" ca="1" si="1">RANDBETWEEN(0, 4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>17150111</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C44" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44468</v>
+      </c>
+      <c r="D44">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>17150028</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44717</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>18150139</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45034</v>
+      </c>
+      <c r="D46">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>14150503</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C47" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44829</v>
+      </c>
+      <c r="D47">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>15151019</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C48" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44378</v>
+      </c>
+      <c r="D48">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>17150029</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45173</v>
+      </c>
+      <c r="D49">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>17150031</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45050</v>
+      </c>
+      <c r="D50">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>18150193</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44324</v>
+      </c>
+      <c r="D51">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>18150266</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44266</v>
+      </c>
+      <c r="D52">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>15150830</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44958</v>
+      </c>
+      <c r="D53">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>15150004</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C54" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44490</v>
+      </c>
+      <c r="D54">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>17150123</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44813</v>
+      </c>
+      <c r="D55">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>16151459</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44837</v>
+      </c>
+      <c r="D56">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>18150142</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44495</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>16150330</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C58" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44999</v>
+      </c>
+      <c r="D58">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>18150194</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C59" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44378</v>
+      </c>
+      <c r="D59">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>18150196</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C60" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44695</v>
+      </c>
+      <c r="D60">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>17150132</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44777</v>
+      </c>
+      <c r="D61">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>18150198</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C62" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45041</v>
+      </c>
+      <c r="D62">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>18150199</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44718</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>16150116</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44281</v>
+      </c>
+      <c r="D64">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>18150202</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44918</v>
+      </c>
+      <c r="D65">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>16150180</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45192</v>
+      </c>
+      <c r="D66">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>16150776</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C67" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45185</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>17150150</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C68" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44776</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>16150120</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C69" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44276</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>15151042</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45265</v>
+      </c>
+      <c r="D70">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>18150206</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C71" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44291</v>
+      </c>
+      <c r="D71">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>16151466</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44524</v>
+      </c>
+      <c r="D72">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>17150342</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C73" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44552</v>
+      </c>
+      <c r="D73">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>17150049</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C74" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45185</v>
+      </c>
+      <c r="D74">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>15151183</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44732</v>
+      </c>
+      <c r="D75">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>16151649</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44740</v>
+      </c>
+      <c r="D76">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>17150163</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C77" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44198</v>
+      </c>
+      <c r="D77">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>17150052</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C78" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44210</v>
+      </c>
+      <c r="D78">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>18150208</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C79" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44515</v>
+      </c>
+      <c r="D79">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>16150190</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C80" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45145</v>
+      </c>
+      <c r="D80">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>17150504</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C81" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44613</v>
+      </c>
+      <c r="D81">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>16150345</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C82" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44957</v>
+      </c>
+      <c r="D82">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>18150211</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C83" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>45091</v>
+      </c>
+      <c r="D83">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>18150212</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C84" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44516</v>
+      </c>
+      <c r="D84">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4290,10 +5395,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4301,7 +5406,7 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
@@ -4317,7 +5422,7 @@
       <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E1" t="s">
@@ -4443,6 +5548,1739 @@
       </c>
       <c r="G6">
         <v>17150005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1111115</v>
+      </c>
+      <c r="B7" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D7" s="1">
+        <v>36859</v>
+      </c>
+      <c r="E7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F7">
+        <v>957525471</v>
+      </c>
+      <c r="G7">
+        <v>18150230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1111116</v>
+      </c>
+      <c r="B8" t="s">
+        <v>233</v>
+      </c>
+      <c r="C8" t="s">
+        <v>312</v>
+      </c>
+      <c r="D8" s="1">
+        <v>36647</v>
+      </c>
+      <c r="E8" t="s">
+        <v>334</v>
+      </c>
+      <c r="F8">
+        <v>1517936087</v>
+      </c>
+      <c r="G8">
+        <v>18150169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1111117</v>
+      </c>
+      <c r="B9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" t="s">
+        <v>313</v>
+      </c>
+      <c r="D9" s="1">
+        <v>36841</v>
+      </c>
+      <c r="E9" t="s">
+        <v>335</v>
+      </c>
+      <c r="F9">
+        <v>905243600</v>
+      </c>
+      <c r="G9">
+        <v>18150232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1111118</v>
+      </c>
+      <c r="B10" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" t="s">
+        <v>312</v>
+      </c>
+      <c r="D10" s="1">
+        <v>36811</v>
+      </c>
+      <c r="E10" t="s">
+        <v>336</v>
+      </c>
+      <c r="F10">
+        <v>979012411</v>
+      </c>
+      <c r="G10">
+        <v>18150172</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1111119</v>
+      </c>
+      <c r="B11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" t="s">
+        <v>312</v>
+      </c>
+      <c r="D11" s="1">
+        <v>36781</v>
+      </c>
+      <c r="E11" t="s">
+        <v>337</v>
+      </c>
+      <c r="F11">
+        <v>989950469</v>
+      </c>
+      <c r="G11">
+        <v>18150173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1111120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" t="s">
+        <v>312</v>
+      </c>
+      <c r="D12" s="1">
+        <v>36789</v>
+      </c>
+      <c r="E12" t="s">
+        <v>338</v>
+      </c>
+      <c r="F12">
+        <v>989970469</v>
+      </c>
+      <c r="G12">
+        <v>18150174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1111121</v>
+      </c>
+      <c r="B13" t="s">
+        <v>238</v>
+      </c>
+      <c r="C13" t="s">
+        <v>311</v>
+      </c>
+      <c r="D13" s="1">
+        <v>36843</v>
+      </c>
+      <c r="E13" t="s">
+        <v>339</v>
+      </c>
+      <c r="G13">
+        <v>18150233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1111122</v>
+      </c>
+      <c r="B14" t="s">
+        <v>239</v>
+      </c>
+      <c r="C14" t="s">
+        <v>312</v>
+      </c>
+      <c r="D14" s="1">
+        <v>36777</v>
+      </c>
+      <c r="E14" t="s">
+        <v>340</v>
+      </c>
+      <c r="G14">
+        <v>18150171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1111123</v>
+      </c>
+      <c r="B15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C15" t="s">
+        <v>313</v>
+      </c>
+      <c r="D15" s="1">
+        <v>36830</v>
+      </c>
+      <c r="E15" t="s">
+        <v>341</v>
+      </c>
+      <c r="G15">
+        <v>18150234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1111124</v>
+      </c>
+      <c r="B16" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" t="s">
+        <v>311</v>
+      </c>
+      <c r="D16" s="1">
+        <v>36613</v>
+      </c>
+      <c r="E16" t="s">
+        <v>342</v>
+      </c>
+      <c r="F16">
+        <v>972755453</v>
+      </c>
+      <c r="G16">
+        <v>18150238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1111125</v>
+      </c>
+      <c r="B17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="1">
+        <v>36258</v>
+      </c>
+      <c r="E17" t="s">
+        <v>343</v>
+      </c>
+      <c r="G17">
+        <v>17150003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1111126</v>
+      </c>
+      <c r="B18" t="s">
+        <v>243</v>
+      </c>
+      <c r="C18" t="s">
+        <v>314</v>
+      </c>
+      <c r="D18" s="1">
+        <v>36233</v>
+      </c>
+      <c r="E18" t="s">
+        <v>344</v>
+      </c>
+      <c r="F18">
+        <v>983853567</v>
+      </c>
+      <c r="G18">
+        <v>17150085</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1111127</v>
+      </c>
+      <c r="B19" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" t="s">
+        <v>312</v>
+      </c>
+      <c r="D19" s="1">
+        <v>36478</v>
+      </c>
+      <c r="E19" t="s">
+        <v>345</v>
+      </c>
+      <c r="F19">
+        <v>915361779</v>
+      </c>
+      <c r="G19">
+        <v>18150175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1111128</v>
+      </c>
+      <c r="B20" t="s">
+        <v>245</v>
+      </c>
+      <c r="C20" t="s">
+        <v>315</v>
+      </c>
+      <c r="D20" s="1">
+        <v>36014</v>
+      </c>
+      <c r="E20" t="s">
+        <v>346</v>
+      </c>
+      <c r="G20">
+        <v>16150084</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1111129</v>
+      </c>
+      <c r="B21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" t="s">
+        <v>312</v>
+      </c>
+      <c r="D21" s="1">
+        <v>36739</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21">
+        <v>18150179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1111130</v>
+      </c>
+      <c r="B22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C22" t="s">
+        <v>316</v>
+      </c>
+      <c r="D22" s="1">
+        <v>35870</v>
+      </c>
+      <c r="E22" t="s">
+        <v>347</v>
+      </c>
+      <c r="G22">
+        <v>16150229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1111131</v>
+      </c>
+      <c r="B23" t="s">
+        <v>248</v>
+      </c>
+      <c r="C23" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" s="1">
+        <v>35590</v>
+      </c>
+      <c r="E23" t="s">
+        <v>348</v>
+      </c>
+      <c r="G23">
+        <v>15150015</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1111132</v>
+      </c>
+      <c r="B24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C24" t="s">
+        <v>318</v>
+      </c>
+      <c r="D24" s="1">
+        <v>36716</v>
+      </c>
+      <c r="E24" t="s">
+        <v>349</v>
+      </c>
+      <c r="F24">
+        <v>905629639</v>
+      </c>
+      <c r="G24">
+        <v>18150123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>1111133</v>
+      </c>
+      <c r="B25" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" t="s">
+        <v>312</v>
+      </c>
+      <c r="D25" s="1">
+        <v>36803</v>
+      </c>
+      <c r="E25" t="s">
+        <v>350</v>
+      </c>
+      <c r="G25">
+        <v>18150187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1111134</v>
+      </c>
+      <c r="B26" t="s">
+        <v>251</v>
+      </c>
+      <c r="C26" t="s">
+        <v>312</v>
+      </c>
+      <c r="D26" s="1">
+        <v>36865</v>
+      </c>
+      <c r="E26" t="s">
+        <v>338</v>
+      </c>
+      <c r="F26">
+        <v>977103776</v>
+      </c>
+      <c r="G26">
+        <v>18150188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1111135</v>
+      </c>
+      <c r="B27" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" t="s">
+        <v>312</v>
+      </c>
+      <c r="D27" s="1">
+        <v>36706</v>
+      </c>
+      <c r="E27" t="s">
+        <v>351</v>
+      </c>
+      <c r="F27">
+        <v>979024505</v>
+      </c>
+      <c r="G27">
+        <v>18150185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1111136</v>
+      </c>
+      <c r="B28" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" t="s">
+        <v>314</v>
+      </c>
+      <c r="D28" s="1">
+        <v>36487</v>
+      </c>
+      <c r="E28" t="s">
+        <v>352</v>
+      </c>
+      <c r="G28">
+        <v>17151004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1111137</v>
+      </c>
+      <c r="B29" t="s">
+        <v>254</v>
+      </c>
+      <c r="C29" t="s">
+        <v>311</v>
+      </c>
+      <c r="D29" s="1">
+        <v>36584</v>
+      </c>
+      <c r="E29" t="s">
+        <v>353</v>
+      </c>
+      <c r="F29">
+        <v>905484808</v>
+      </c>
+      <c r="G29">
+        <v>18150248</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1111138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" t="s">
+        <v>313</v>
+      </c>
+      <c r="D30" s="1">
+        <v>36720</v>
+      </c>
+      <c r="E30" t="s">
+        <v>335</v>
+      </c>
+      <c r="F30">
+        <v>905484808</v>
+      </c>
+      <c r="G30">
+        <v>18150249</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1111139</v>
+      </c>
+      <c r="B31" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" t="s">
+        <v>312</v>
+      </c>
+      <c r="D31" s="1">
+        <v>36662</v>
+      </c>
+      <c r="E31" t="s">
+        <v>342</v>
+      </c>
+      <c r="F31">
+        <v>984864072</v>
+      </c>
+      <c r="G31">
+        <v>18150181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1111140</v>
+      </c>
+      <c r="B32" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="1">
+        <v>36247</v>
+      </c>
+      <c r="E32" t="s">
+        <v>333</v>
+      </c>
+      <c r="G32">
+        <v>17150008</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1111141</v>
+      </c>
+      <c r="B33" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" t="s">
+        <v>319</v>
+      </c>
+      <c r="D33" s="1">
+        <v>36203</v>
+      </c>
+      <c r="E33" t="s">
+        <v>344</v>
+      </c>
+      <c r="F33">
+        <v>1685349007</v>
+      </c>
+      <c r="G33">
+        <v>17150424</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>1111142</v>
+      </c>
+      <c r="B34" t="s">
+        <v>259</v>
+      </c>
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="1">
+        <v>36468</v>
+      </c>
+      <c r="E34" t="s">
+        <v>354</v>
+      </c>
+      <c r="G34">
+        <v>17150010</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>1111143</v>
+      </c>
+      <c r="B35" t="s">
+        <v>260</v>
+      </c>
+      <c r="C35" t="s">
+        <v>312</v>
+      </c>
+      <c r="D35" s="1">
+        <v>36556</v>
+      </c>
+      <c r="E35" t="s">
+        <v>355</v>
+      </c>
+      <c r="F35">
+        <v>1234377007</v>
+      </c>
+      <c r="G35">
+        <v>18150183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1111144</v>
+      </c>
+      <c r="B36" t="s">
+        <v>261</v>
+      </c>
+      <c r="C36" t="s">
+        <v>311</v>
+      </c>
+      <c r="D36" s="1">
+        <v>36612</v>
+      </c>
+      <c r="E36" t="s">
+        <v>356</v>
+      </c>
+      <c r="G36">
+        <v>18150246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1111145</v>
+      </c>
+      <c r="B37" t="s">
+        <v>262</v>
+      </c>
+      <c r="C37" t="s">
+        <v>312</v>
+      </c>
+      <c r="D37" s="1">
+        <v>36851</v>
+      </c>
+      <c r="E37" t="s">
+        <v>340</v>
+      </c>
+      <c r="F37">
+        <v>905669673</v>
+      </c>
+      <c r="G37">
+        <v>18150189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1111146</v>
+      </c>
+      <c r="B38" t="s">
+        <v>263</v>
+      </c>
+      <c r="C38" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="1">
+        <v>36198</v>
+      </c>
+      <c r="E38" t="s">
+        <v>357</v>
+      </c>
+      <c r="F38">
+        <v>979793396</v>
+      </c>
+      <c r="G38">
+        <v>17150020</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1111147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>264</v>
+      </c>
+      <c r="C39" t="s">
+        <v>312</v>
+      </c>
+      <c r="D39" s="1">
+        <v>36839</v>
+      </c>
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39">
+        <v>982005331</v>
+      </c>
+      <c r="G39">
+        <v>18150190</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1111148</v>
+      </c>
+      <c r="B40" t="s">
+        <v>265</v>
+      </c>
+      <c r="C40" t="s">
+        <v>315</v>
+      </c>
+      <c r="D40" s="1">
+        <v>35850</v>
+      </c>
+      <c r="E40" t="s">
+        <v>358</v>
+      </c>
+      <c r="F40">
+        <v>915003445</v>
+      </c>
+      <c r="G40">
+        <v>16150100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1111149</v>
+      </c>
+      <c r="B41" t="s">
+        <v>266</v>
+      </c>
+      <c r="C41" t="s">
+        <v>311</v>
+      </c>
+      <c r="D41" s="1">
+        <v>36709</v>
+      </c>
+      <c r="E41" t="s">
+        <v>359</v>
+      </c>
+      <c r="F41">
+        <v>935228199</v>
+      </c>
+      <c r="G41">
+        <v>18150255</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1111150</v>
+      </c>
+      <c r="B42" t="s">
+        <v>267</v>
+      </c>
+      <c r="C42" t="s">
+        <v>313</v>
+      </c>
+      <c r="D42" s="1">
+        <v>36651</v>
+      </c>
+      <c r="E42" t="s">
+        <v>360</v>
+      </c>
+      <c r="G42">
+        <v>18150256</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1111151</v>
+      </c>
+      <c r="B43" t="s">
+        <v>268</v>
+      </c>
+      <c r="C43" t="s">
+        <v>311</v>
+      </c>
+      <c r="D43" s="1">
+        <v>36831</v>
+      </c>
+      <c r="E43" t="s">
+        <v>361</v>
+      </c>
+      <c r="G43">
+        <v>18150257</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1111152</v>
+      </c>
+      <c r="B44" t="s">
+        <v>269</v>
+      </c>
+      <c r="C44" t="s">
+        <v>320</v>
+      </c>
+      <c r="D44" s="1">
+        <v>36484</v>
+      </c>
+      <c r="E44" t="s">
+        <v>362</v>
+      </c>
+      <c r="G44">
+        <v>17151003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1111153</v>
+      </c>
+      <c r="B45" t="s">
+        <v>270</v>
+      </c>
+      <c r="C45" t="s">
+        <v>314</v>
+      </c>
+      <c r="D45" s="1">
+        <v>36162</v>
+      </c>
+      <c r="E45" t="s">
+        <v>363</v>
+      </c>
+      <c r="G45">
+        <v>17150111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1111154</v>
+      </c>
+      <c r="B46" t="s">
+        <v>271</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="1">
+        <v>36467</v>
+      </c>
+      <c r="E46" t="s">
+        <v>339</v>
+      </c>
+      <c r="F46" t="s">
+        <v>330</v>
+      </c>
+      <c r="G46">
+        <v>17150028</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1111155</v>
+      </c>
+      <c r="B47" t="s">
+        <v>272</v>
+      </c>
+      <c r="C47" t="s">
+        <v>318</v>
+      </c>
+      <c r="D47" s="1">
+        <v>36766</v>
+      </c>
+      <c r="E47" t="s">
+        <v>347</v>
+      </c>
+      <c r="G47">
+        <v>18150139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1111156</v>
+      </c>
+      <c r="B48" t="s">
+        <v>273</v>
+      </c>
+      <c r="C48" t="s">
+        <v>321</v>
+      </c>
+      <c r="D48" s="1">
+        <v>35185</v>
+      </c>
+      <c r="E48" t="s">
+        <v>338</v>
+      </c>
+      <c r="F48">
+        <v>935056206</v>
+      </c>
+      <c r="G48">
+        <v>14150503</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>1111157</v>
+      </c>
+      <c r="B49" t="s">
+        <v>274</v>
+      </c>
+      <c r="C49" t="s">
+        <v>322</v>
+      </c>
+      <c r="D49" s="1">
+        <v>35511</v>
+      </c>
+      <c r="E49" t="s">
+        <v>360</v>
+      </c>
+      <c r="F49">
+        <v>933540599</v>
+      </c>
+      <c r="G49">
+        <v>15151019</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1111158</v>
+      </c>
+      <c r="B50" t="s">
+        <v>275</v>
+      </c>
+      <c r="C50" t="s">
+        <v>94</v>
+      </c>
+      <c r="D50" s="1">
+        <v>36364</v>
+      </c>
+      <c r="E50" t="s">
+        <v>363</v>
+      </c>
+      <c r="G50">
+        <v>17150029</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1111159</v>
+      </c>
+      <c r="B51" t="s">
+        <v>276</v>
+      </c>
+      <c r="C51" t="s">
+        <v>94</v>
+      </c>
+      <c r="D51" s="1">
+        <v>36416</v>
+      </c>
+      <c r="E51" t="s">
+        <v>364</v>
+      </c>
+      <c r="F51">
+        <v>988201498</v>
+      </c>
+      <c r="G51">
+        <v>17150031</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>1111160</v>
+      </c>
+      <c r="B52" t="s">
+        <v>277</v>
+      </c>
+      <c r="C52" t="s">
+        <v>312</v>
+      </c>
+      <c r="D52" s="1">
+        <v>36771</v>
+      </c>
+      <c r="E52" t="s">
+        <v>365</v>
+      </c>
+      <c r="F52">
+        <v>935454511</v>
+      </c>
+      <c r="G52">
+        <v>18150193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>1111161</v>
+      </c>
+      <c r="B53" t="s">
+        <v>278</v>
+      </c>
+      <c r="C53" t="s">
+        <v>311</v>
+      </c>
+      <c r="D53" s="1">
+        <v>36690</v>
+      </c>
+      <c r="E53" t="s">
+        <v>334</v>
+      </c>
+      <c r="F53">
+        <v>946186886</v>
+      </c>
+      <c r="G53">
+        <v>18150266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>1111162</v>
+      </c>
+      <c r="B54" t="s">
+        <v>279</v>
+      </c>
+      <c r="C54" t="s">
+        <v>332</v>
+      </c>
+      <c r="D54" s="1">
+        <v>35506</v>
+      </c>
+      <c r="E54" t="s">
+        <v>338</v>
+      </c>
+      <c r="F54" t="s">
+        <v>331</v>
+      </c>
+      <c r="G54">
+        <v>15150830</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>1111163</v>
+      </c>
+      <c r="B55" t="s">
+        <v>280</v>
+      </c>
+      <c r="C55" t="s">
+        <v>317</v>
+      </c>
+      <c r="D55" s="1">
+        <v>35456</v>
+      </c>
+      <c r="E55" t="s">
+        <v>344</v>
+      </c>
+      <c r="F55">
+        <v>915301065</v>
+      </c>
+      <c r="G55">
+        <v>15150004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>1111164</v>
+      </c>
+      <c r="B56" t="s">
+        <v>281</v>
+      </c>
+      <c r="C56" t="s">
+        <v>314</v>
+      </c>
+      <c r="D56" s="1">
+        <v>36392</v>
+      </c>
+      <c r="E56" t="s">
+        <v>338</v>
+      </c>
+      <c r="F56">
+        <v>983799417</v>
+      </c>
+      <c r="G56">
+        <v>17150123</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>1111165</v>
+      </c>
+      <c r="B57" t="s">
+        <v>282</v>
+      </c>
+      <c r="C57" t="s">
+        <v>323</v>
+      </c>
+      <c r="D57" s="1">
+        <v>35810</v>
+      </c>
+      <c r="E57" t="s">
+        <v>366</v>
+      </c>
+      <c r="F57">
+        <v>1224207990</v>
+      </c>
+      <c r="G57">
+        <v>16151459</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1111166</v>
+      </c>
+      <c r="B58" t="s">
+        <v>283</v>
+      </c>
+      <c r="C58" t="s">
+        <v>318</v>
+      </c>
+      <c r="D58" s="1">
+        <v>36563</v>
+      </c>
+      <c r="E58" t="s">
+        <v>356</v>
+      </c>
+      <c r="F58">
+        <v>1666461274</v>
+      </c>
+      <c r="G58">
+        <v>18150142</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>1111167</v>
+      </c>
+      <c r="B59" t="s">
+        <v>284</v>
+      </c>
+      <c r="C59" t="s">
+        <v>324</v>
+      </c>
+      <c r="D59" s="1">
+        <v>36108</v>
+      </c>
+      <c r="E59" t="s">
+        <v>367</v>
+      </c>
+      <c r="F59">
+        <v>914033933</v>
+      </c>
+      <c r="G59">
+        <v>16150330</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>1111168</v>
+      </c>
+      <c r="B60" t="s">
+        <v>285</v>
+      </c>
+      <c r="C60" t="s">
+        <v>312</v>
+      </c>
+      <c r="D60" s="1">
+        <v>36544</v>
+      </c>
+      <c r="E60" t="s">
+        <v>343</v>
+      </c>
+      <c r="F60">
+        <v>919083637</v>
+      </c>
+      <c r="G60">
+        <v>18150194</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>1111169</v>
+      </c>
+      <c r="B61" t="s">
+        <v>286</v>
+      </c>
+      <c r="C61" t="s">
+        <v>312</v>
+      </c>
+      <c r="D61" s="1">
+        <v>36776</v>
+      </c>
+      <c r="E61" t="s">
+        <v>368</v>
+      </c>
+      <c r="F61">
+        <v>989638138</v>
+      </c>
+      <c r="G61">
+        <v>18150196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1111170</v>
+      </c>
+      <c r="B62" t="s">
+        <v>287</v>
+      </c>
+      <c r="C62" t="s">
+        <v>320</v>
+      </c>
+      <c r="D62" s="1">
+        <v>36342</v>
+      </c>
+      <c r="E62" t="s">
+        <v>369</v>
+      </c>
+      <c r="F62">
+        <v>979810948</v>
+      </c>
+      <c r="G62">
+        <v>17150132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1111171</v>
+      </c>
+      <c r="B63" t="s">
+        <v>288</v>
+      </c>
+      <c r="C63" t="s">
+        <v>312</v>
+      </c>
+      <c r="D63" s="1">
+        <v>36588</v>
+      </c>
+      <c r="E63" t="s">
+        <v>365</v>
+      </c>
+      <c r="G63">
+        <v>18150198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1111172</v>
+      </c>
+      <c r="B64" t="s">
+        <v>289</v>
+      </c>
+      <c r="C64" t="s">
+        <v>312</v>
+      </c>
+      <c r="D64" s="1">
+        <v>36689</v>
+      </c>
+      <c r="E64" t="s">
+        <v>333</v>
+      </c>
+      <c r="F64">
+        <v>1686688723</v>
+      </c>
+      <c r="G64">
+        <v>18150199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>1111173</v>
+      </c>
+      <c r="B65" t="s">
+        <v>290</v>
+      </c>
+      <c r="C65" t="s">
+        <v>315</v>
+      </c>
+      <c r="D65" s="1">
+        <v>35500</v>
+      </c>
+      <c r="E65" t="s">
+        <v>370</v>
+      </c>
+      <c r="F65">
+        <v>915050122</v>
+      </c>
+      <c r="G65">
+        <v>16150116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>1111174</v>
+      </c>
+      <c r="B66" t="s">
+        <v>291</v>
+      </c>
+      <c r="C66" t="s">
+        <v>312</v>
+      </c>
+      <c r="D66" s="1">
+        <v>36773</v>
+      </c>
+      <c r="E66" t="s">
+        <v>365</v>
+      </c>
+      <c r="F66">
+        <v>914979516</v>
+      </c>
+      <c r="G66">
+        <v>18150202</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>1111175</v>
+      </c>
+      <c r="B67" t="s">
+        <v>292</v>
+      </c>
+      <c r="C67" t="s">
+        <v>323</v>
+      </c>
+      <c r="D67" s="1">
+        <v>35886</v>
+      </c>
+      <c r="E67" t="s">
+        <v>349</v>
+      </c>
+      <c r="F67">
+        <v>972624052</v>
+      </c>
+      <c r="G67">
+        <v>16150180</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>1111176</v>
+      </c>
+      <c r="B68" t="s">
+        <v>293</v>
+      </c>
+      <c r="C68" t="s">
+        <v>325</v>
+      </c>
+      <c r="D68" s="1">
+        <v>36007</v>
+      </c>
+      <c r="E68" t="s">
+        <v>336</v>
+      </c>
+      <c r="F68">
+        <v>983211135</v>
+      </c>
+      <c r="G68">
+        <v>16150776</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>1111177</v>
+      </c>
+      <c r="B69" t="s">
+        <v>294</v>
+      </c>
+      <c r="C69" t="s">
+        <v>320</v>
+      </c>
+      <c r="D69" s="1">
+        <v>36441</v>
+      </c>
+      <c r="E69" t="s">
+        <v>365</v>
+      </c>
+      <c r="G69">
+        <v>17150150</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>1111178</v>
+      </c>
+      <c r="B70" t="s">
+        <v>295</v>
+      </c>
+      <c r="C70" t="s">
+        <v>315</v>
+      </c>
+      <c r="D70" s="1">
+        <v>35922</v>
+      </c>
+      <c r="E70" t="s">
+        <v>333</v>
+      </c>
+      <c r="F70">
+        <v>942113606</v>
+      </c>
+      <c r="G70">
+        <v>16150120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1111179</v>
+      </c>
+      <c r="B71" t="s">
+        <v>296</v>
+      </c>
+      <c r="C71" t="s">
+        <v>326</v>
+      </c>
+      <c r="D71" s="1">
+        <v>35724</v>
+      </c>
+      <c r="E71" t="s">
+        <v>334</v>
+      </c>
+      <c r="G71">
+        <v>15151042</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1111180</v>
+      </c>
+      <c r="B72" t="s">
+        <v>297</v>
+      </c>
+      <c r="C72" t="s">
+        <v>312</v>
+      </c>
+      <c r="D72" s="1">
+        <v>36805</v>
+      </c>
+      <c r="E72" t="s">
+        <v>335</v>
+      </c>
+      <c r="F72">
+        <v>917679396</v>
+      </c>
+      <c r="G72">
+        <v>18150206</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>1111181</v>
+      </c>
+      <c r="B73" t="s">
+        <v>298</v>
+      </c>
+      <c r="C73" t="s">
+        <v>323</v>
+      </c>
+      <c r="D73" s="1">
+        <v>35850</v>
+      </c>
+      <c r="E73" t="s">
+        <v>336</v>
+      </c>
+      <c r="G73">
+        <v>16151466</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>1111182</v>
+      </c>
+      <c r="B74" t="s">
+        <v>299</v>
+      </c>
+      <c r="C74" t="s">
+        <v>327</v>
+      </c>
+      <c r="D74" s="1">
+        <v>36458</v>
+      </c>
+      <c r="E74" t="s">
+        <v>337</v>
+      </c>
+      <c r="F74">
+        <v>905257433</v>
+      </c>
+      <c r="G74">
+        <v>17150342</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>1111183</v>
+      </c>
+      <c r="B75" t="s">
+        <v>300</v>
+      </c>
+      <c r="C75" t="s">
+        <v>94</v>
+      </c>
+      <c r="D75" s="1">
+        <v>36328</v>
+      </c>
+      <c r="E75" t="s">
+        <v>338</v>
+      </c>
+      <c r="F75">
+        <v>988616588</v>
+      </c>
+      <c r="G75">
+        <v>17150049</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>1111184</v>
+      </c>
+      <c r="B76" t="s">
+        <v>301</v>
+      </c>
+      <c r="C76" t="s">
+        <v>328</v>
+      </c>
+      <c r="D76" s="1">
+        <v>35686</v>
+      </c>
+      <c r="E76" t="s">
+        <v>339</v>
+      </c>
+      <c r="G76">
+        <v>15151183</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>1111185</v>
+      </c>
+      <c r="B77" t="s">
+        <v>302</v>
+      </c>
+      <c r="C77" t="s">
+        <v>315</v>
+      </c>
+      <c r="D77" s="1">
+        <v>35817</v>
+      </c>
+      <c r="E77" t="s">
+        <v>340</v>
+      </c>
+      <c r="G77">
+        <v>16151649</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>1111186</v>
+      </c>
+      <c r="B78" t="s">
+        <v>303</v>
+      </c>
+      <c r="C78" t="s">
+        <v>314</v>
+      </c>
+      <c r="D78" s="1">
+        <v>36301</v>
+      </c>
+      <c r="E78" t="s">
+        <v>341</v>
+      </c>
+      <c r="F78">
+        <v>919611828</v>
+      </c>
+      <c r="G78">
+        <v>17150163</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>1111187</v>
+      </c>
+      <c r="B79" t="s">
+        <v>304</v>
+      </c>
+      <c r="C79" t="s">
+        <v>94</v>
+      </c>
+      <c r="D79" s="1">
+        <v>36264</v>
+      </c>
+      <c r="E79" t="s">
+        <v>342</v>
+      </c>
+      <c r="G79">
+        <v>17150052</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>1111188</v>
+      </c>
+      <c r="B80" t="s">
+        <v>305</v>
+      </c>
+      <c r="C80" t="s">
+        <v>312</v>
+      </c>
+      <c r="D80" s="1">
+        <v>36679</v>
+      </c>
+      <c r="E80" t="s">
+        <v>343</v>
+      </c>
+      <c r="F80">
+        <v>948192263</v>
+      </c>
+      <c r="G80">
+        <v>18150208</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>1111189</v>
+      </c>
+      <c r="B81" t="s">
+        <v>306</v>
+      </c>
+      <c r="C81" t="s">
+        <v>323</v>
+      </c>
+      <c r="D81" s="1">
+        <v>36066</v>
+      </c>
+      <c r="E81" t="s">
+        <v>344</v>
+      </c>
+      <c r="F81">
+        <v>914111707</v>
+      </c>
+      <c r="G81">
+        <v>16150190</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>1111190</v>
+      </c>
+      <c r="B82" t="s">
+        <v>307</v>
+      </c>
+      <c r="C82" t="s">
+        <v>319</v>
+      </c>
+      <c r="D82" s="1">
+        <v>36319</v>
+      </c>
+      <c r="E82" t="s">
+        <v>345</v>
+      </c>
+      <c r="G82">
+        <v>17150504</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>1111191</v>
+      </c>
+      <c r="B83" t="s">
+        <v>308</v>
+      </c>
+      <c r="C83" t="s">
+        <v>329</v>
+      </c>
+      <c r="D83" s="1">
+        <v>36126</v>
+      </c>
+      <c r="E83" t="s">
+        <v>346</v>
+      </c>
+      <c r="F83">
+        <v>914145414</v>
+      </c>
+      <c r="G83">
+        <v>16150345</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>1111192</v>
+      </c>
+      <c r="B84" t="s">
+        <v>309</v>
+      </c>
+      <c r="C84" t="s">
+        <v>312</v>
+      </c>
+      <c r="D84" s="1">
+        <v>36593</v>
+      </c>
+      <c r="E84" t="s">
+        <v>97</v>
+      </c>
+      <c r="G84">
+        <v>18150211</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>1111193</v>
+      </c>
+      <c r="B85" t="s">
+        <v>310</v>
+      </c>
+      <c r="C85" t="s">
+        <v>312</v>
+      </c>
+      <c r="D85" s="1">
+        <v>36774</v>
+      </c>
+      <c r="E85" t="s">
+        <v>347</v>
+      </c>
+      <c r="F85">
+        <v>982191252</v>
+      </c>
+      <c r="G85">
+        <v>18150212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lực thêm 1 vài câu sql chức năng
</commit_message>
<xml_diff>
--- a/TTCSDL.xlsx
+++ b/TTCSDL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="630" yWindow="345" windowWidth="20940" windowHeight="9870" tabRatio="896" firstSheet="12" activeTab="19"/>
+    <workbookView xWindow="630" yWindow="345" windowWidth="20940" windowHeight="9870" tabRatio="896" firstSheet="13" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="TACGIA" sheetId="1" r:id="rId1"/>
@@ -2430,11 +2430,11 @@
       </c>
       <c r="B7" s="1">
         <f ca="1">RANDBETWEEN(DATE(2020,2,1),DATE(2020,3,31))</f>
-        <v>43876</v>
+        <v>43917</v>
       </c>
       <c r="C7" s="1">
         <f ca="1">RANDBETWEEN(DATE(2020,4,1),DATE(2020,5,31))</f>
-        <v>43964</v>
+        <v>43922</v>
       </c>
       <c r="D7" s="19">
         <v>18150230</v>
@@ -2446,11 +2446,11 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ref="B8:B41" ca="1" si="0">RANDBETWEEN(DATE(2020,2,1),DATE(2020,3,31))</f>
-        <v>43902</v>
+        <v>43917</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ref="C8:C41" ca="1" si="1">RANDBETWEEN(DATE(2020,4,1),DATE(2020,5,31))</f>
-        <v>43937</v>
+        <v>43974</v>
       </c>
       <c r="D8" s="19">
         <v>18150169</v>
@@ -2462,11 +2462,11 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43885</v>
+        <v>43898</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43975</v>
+        <v>43945</v>
       </c>
       <c r="D9" s="19">
         <v>18150232</v>
@@ -2478,11 +2478,11 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43892</v>
+        <v>43880</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43975</v>
+        <v>43958</v>
       </c>
       <c r="D10" s="19">
         <v>18150172</v>
@@ -2494,11 +2494,11 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43886</v>
+        <v>43881</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43968</v>
+        <v>43949</v>
       </c>
       <c r="D11" s="19">
         <v>18150173</v>
@@ -2514,7 +2514,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43943</v>
+        <v>43979</v>
       </c>
       <c r="D12" s="19">
         <v>18150174</v>
@@ -2526,11 +2526,11 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43884</v>
+        <v>43888</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43956</v>
+        <v>43960</v>
       </c>
       <c r="D13" s="19">
         <v>18150233</v>
@@ -2542,11 +2542,11 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43865</v>
+        <v>43896</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43940</v>
+        <v>43945</v>
       </c>
       <c r="D14">
         <v>18150171</v>
@@ -2558,11 +2558,11 @@
       </c>
       <c r="B15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43864</v>
+        <v>43895</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43954</v>
+        <v>43949</v>
       </c>
       <c r="D15">
         <v>18150234</v>
@@ -2574,11 +2574,11 @@
       </c>
       <c r="B16" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43869</v>
+        <v>43906</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43964</v>
+        <v>43937</v>
       </c>
       <c r="D16">
         <v>18150238</v>
@@ -2590,11 +2590,11 @@
       </c>
       <c r="B17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43906</v>
+        <v>43866</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43972</v>
+        <v>43959</v>
       </c>
       <c r="D17">
         <v>17150003</v>
@@ -2606,11 +2606,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43901</v>
+        <v>43899</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43930</v>
+        <v>43937</v>
       </c>
       <c r="D18">
         <v>17150085</v>
@@ -2622,11 +2622,11 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43887</v>
+        <v>43910</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43937</v>
+        <v>43928</v>
       </c>
       <c r="D19">
         <v>18150175</v>
@@ -2638,11 +2638,11 @@
       </c>
       <c r="B20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43901</v>
+        <v>43867</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43952</v>
+        <v>43948</v>
       </c>
       <c r="D20">
         <v>16150084</v>
@@ -2654,11 +2654,11 @@
       </c>
       <c r="B21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43866</v>
+        <v>43871</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43978</v>
+        <v>43943</v>
       </c>
       <c r="D21">
         <v>18150179</v>
@@ -2670,11 +2670,11 @@
       </c>
       <c r="B22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43881</v>
+        <v>43864</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43934</v>
+        <v>43980</v>
       </c>
       <c r="D22">
         <v>16150229</v>
@@ -2686,11 +2686,11 @@
       </c>
       <c r="B23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43912</v>
+        <v>43898</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43922</v>
+        <v>43977</v>
       </c>
       <c r="D23">
         <v>15150015</v>
@@ -2702,11 +2702,11 @@
       </c>
       <c r="B24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43885</v>
+        <v>43867</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43952</v>
+        <v>43925</v>
       </c>
       <c r="D24">
         <v>18150123</v>
@@ -2718,11 +2718,11 @@
       </c>
       <c r="B25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43874</v>
+        <v>43887</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43965</v>
+        <v>43971</v>
       </c>
       <c r="D25">
         <v>18150187</v>
@@ -2734,11 +2734,11 @@
       </c>
       <c r="B26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43892</v>
+        <v>43864</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43971</v>
+        <v>43974</v>
       </c>
       <c r="D26">
         <v>18150188</v>
@@ -2750,11 +2750,11 @@
       </c>
       <c r="B27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43898</v>
+        <v>43901</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43922</v>
+        <v>43963</v>
       </c>
       <c r="D27">
         <v>18150185</v>
@@ -2766,11 +2766,11 @@
       </c>
       <c r="B28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43874</v>
+        <v>43889</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43978</v>
+        <v>43947</v>
       </c>
       <c r="D28">
         <v>17151004</v>
@@ -2782,11 +2782,11 @@
       </c>
       <c r="B29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43906</v>
+        <v>43897</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43937</v>
+        <v>43977</v>
       </c>
       <c r="D29">
         <v>18150248</v>
@@ -2798,11 +2798,11 @@
       </c>
       <c r="B30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43893</v>
+        <v>43899</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43980</v>
+        <v>43960</v>
       </c>
       <c r="D30">
         <v>18150249</v>
@@ -2814,11 +2814,11 @@
       </c>
       <c r="B31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43910</v>
+        <v>43874</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43972</v>
+        <v>43924</v>
       </c>
       <c r="D31">
         <v>18150181</v>
@@ -2830,11 +2830,11 @@
       </c>
       <c r="B32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43901</v>
+        <v>43881</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43966</v>
+        <v>43979</v>
       </c>
       <c r="D32">
         <v>17150008</v>
@@ -2846,11 +2846,11 @@
       </c>
       <c r="B33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43886</v>
+        <v>43894</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43924</v>
+        <v>43950</v>
       </c>
       <c r="D33">
         <v>17150424</v>
@@ -2862,11 +2862,11 @@
       </c>
       <c r="B34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43872</v>
+        <v>43877</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43958</v>
+        <v>43982</v>
       </c>
       <c r="D34">
         <v>17150010</v>
@@ -2878,11 +2878,11 @@
       </c>
       <c r="B35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43897</v>
+        <v>43910</v>
       </c>
       <c r="C35" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43931</v>
+        <v>43950</v>
       </c>
       <c r="D35">
         <v>18150183</v>
@@ -2894,11 +2894,11 @@
       </c>
       <c r="B36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43890</v>
+        <v>43877</v>
       </c>
       <c r="C36" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43925</v>
+        <v>43943</v>
       </c>
       <c r="D36">
         <v>18150246</v>
@@ -2910,11 +2910,11 @@
       </c>
       <c r="B37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43865</v>
+        <v>43870</v>
       </c>
       <c r="C37" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43924</v>
+        <v>43949</v>
       </c>
       <c r="D37">
         <v>18150189</v>
@@ -2926,11 +2926,11 @@
       </c>
       <c r="B38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43904</v>
+        <v>43915</v>
       </c>
       <c r="C38" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43927</v>
+        <v>43925</v>
       </c>
       <c r="D38">
         <v>17150020</v>
@@ -2942,11 +2942,11 @@
       </c>
       <c r="B39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43916</v>
+        <v>43909</v>
       </c>
       <c r="C39" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43966</v>
+        <v>43968</v>
       </c>
       <c r="D39">
         <v>18150190</v>
@@ -2958,11 +2958,11 @@
       </c>
       <c r="B40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43875</v>
+        <v>43886</v>
       </c>
       <c r="C40" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43966</v>
+        <v>43978</v>
       </c>
       <c r="D40">
         <v>16150100</v>
@@ -2974,11 +2974,11 @@
       </c>
       <c r="B41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43882</v>
+        <v>43868</v>
       </c>
       <c r="C41" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43942</v>
+        <v>43978</v>
       </c>
       <c r="D41">
         <v>18150255</v>
@@ -3720,7 +3720,7 @@
       </c>
       <c r="B7" s="1">
         <f ca="1">RANDBETWEEN(DATE(2020,3,31),DATE(2020,4,15))</f>
-        <v>43934</v>
+        <v>43928</v>
       </c>
       <c r="C7">
         <v>18150230</v>
@@ -3731,8 +3731,8 @@
         <v>327</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" ref="B8:B30" ca="1" si="0">RANDBETWEEN(DATE(2020,3,31),DATE(2020,4,15))</f>
-        <v>43934</v>
+        <f t="shared" ref="B8:B13" ca="1" si="0">RANDBETWEEN(DATE(2020,3,31),DATE(2020,4,15))</f>
+        <v>43931</v>
       </c>
       <c r="C8">
         <v>18150169</v>
@@ -3744,7 +3744,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43933</v>
+        <v>43921</v>
       </c>
       <c r="C9">
         <v>18150232</v>
@@ -3756,7 +3756,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43924</v>
+        <v>43935</v>
       </c>
       <c r="C10">
         <v>18150172</v>
@@ -3768,7 +3768,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43931</v>
+        <v>43929</v>
       </c>
       <c r="C11">
         <v>18150173</v>
@@ -3780,7 +3780,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="C12">
         <v>18150174</v>
@@ -3792,7 +3792,7 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43925</v>
+        <v>43921</v>
       </c>
       <c r="C13">
         <v>18150233</v>
@@ -4303,7 +4303,7 @@
       </c>
       <c r="C11">
         <f t="shared" ref="C11" ca="1" si="0">RANDBETWEEN(199, 333)</f>
-        <v>274</v>
+        <v>329</v>
       </c>
       <c r="D11" t="s">
         <v>400</v>
@@ -7267,15 +7267,15 @@
       </c>
       <c r="B7" s="1">
         <f ca="1">RANDBETWEEN(DATE(2020,2,1),DATE(2020,2,31))</f>
-        <v>43878</v>
+        <v>43892</v>
       </c>
       <c r="C7">
         <f t="shared" ref="C7:C13" ca="1" si="0">RANDBETWEEN(200,300)</f>
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="D7">
         <f ca="1">RANDBETWEEN(200,300)</f>
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -7287,15 +7287,15 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" ref="B8:B14" ca="1" si="1">RANDBETWEEN(DATE(2020,2,1),DATE(2020,2,31))</f>
-        <v>43877</v>
+        <v>43872</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>222</v>
+        <v>275</v>
       </c>
       <c r="D8">
         <f t="shared" ref="D8:D14" ca="1" si="2">RANDBETWEEN(200,300)</f>
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -7307,15 +7307,15 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43865</v>
+        <v>43872</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>223</v>
+        <v>291</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
-        <v>259</v>
+        <v>276</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -7327,15 +7327,15 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43862</v>
+        <v>43884</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>284</v>
+        <v>242</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="2"/>
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="E10">
         <v>4</v>
@@ -7347,15 +7347,15 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43882</v>
+        <v>43884</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>294</v>
+        <v>219</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="2"/>
-        <v>212</v>
+        <v>242</v>
       </c>
       <c r="E11">
         <v>5</v>
@@ -7367,15 +7367,15 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43877</v>
+        <v>43882</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="2"/>
-        <v>290</v>
+        <v>227</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -7387,15 +7387,15 @@
       </c>
       <c r="B13" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43872</v>
+        <v>43881</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="2"/>
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="E13">
         <v>5</v>
@@ -7407,15 +7407,15 @@
       </c>
       <c r="B14" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>43862</v>
+        <v>43892</v>
       </c>
       <c r="C14">
         <f ca="1">RANDBETWEEN(200,300)</f>
-        <v>299</v>
+        <v>245</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="2"/>
-        <v>226</v>
+        <v>271</v>
       </c>
       <c r="E14">
         <v>5</v>
@@ -8202,7 +8202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="A14" sqref="A14:B30"/>
     </sheetView>
   </sheetViews>
@@ -8499,7 +8499,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D20" ca="1" si="0">RANDBETWEEN(1,20)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="9">
         <v>91</v>
@@ -8517,7 +8517,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E4" s="9">
         <v>92</v>
@@ -8535,7 +8535,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E5" s="9">
         <v>93</v>
@@ -8554,7 +8554,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E6" s="9">
         <v>94</v>
@@ -8573,7 +8573,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E7" s="9">
         <v>95</v>
@@ -8592,7 +8592,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E8" s="9">
         <v>96</v>
@@ -8611,7 +8611,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E9" s="9">
         <v>97</v>
@@ -8630,7 +8630,7 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E10" s="9">
         <v>98</v>
@@ -8649,7 +8649,7 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E11" s="9">
         <v>99</v>
@@ -8668,7 +8668,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E12" s="9">
         <v>100</v>
@@ -8706,7 +8706,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E14" s="9">
         <v>102</v>
@@ -8725,7 +8725,7 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E15" s="9">
         <v>103</v>
@@ -8744,7 +8744,7 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="9">
         <v>104</v>
@@ -8763,7 +8763,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E17" s="9">
         <v>105</v>
@@ -8801,7 +8801,7 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E19" s="9">
         <v>107</v>
@@ -8820,7 +8820,7 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E20" s="9">
         <v>108</v>
@@ -8854,7 +8854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -8953,7 +8953,7 @@
       </c>
       <c r="C8" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43921</v>
+        <v>43932</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -8965,7 +8965,7 @@
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43927</v>
+        <v>43932</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -8977,7 +8977,7 @@
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43933</v>
+        <v>43934</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -8989,7 +8989,7 @@
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43933</v>
+        <v>43935</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -9013,7 +9013,7 @@
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43935</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -9037,7 +9037,7 @@
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>43929</v>
+        <v>43932</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -10003,8 +10003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84:XFD84"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10346,7 +10346,7 @@
       </c>
       <c r="C24" s="1">
         <f t="shared" ref="C24:C55" ca="1" si="0">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
-        <v>44281</v>
+        <v>44525</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -10361,7 +10361,7 @@
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44673</v>
+        <v>44535</v>
       </c>
       <c r="D25">
         <v>2</v>
@@ -10376,7 +10376,7 @@
       </c>
       <c r="C26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44685</v>
+        <v>45250</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -10391,7 +10391,7 @@
       </c>
       <c r="C27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44823</v>
+        <v>45050</v>
       </c>
       <c r="D27">
         <v>2</v>
@@ -10406,7 +10406,7 @@
       </c>
       <c r="C28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44833</v>
+        <v>45054</v>
       </c>
       <c r="D28">
         <v>2</v>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="C29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44522</v>
+        <v>44724</v>
       </c>
       <c r="D29">
         <v>2</v>
@@ -10436,7 +10436,7 @@
       </c>
       <c r="C30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44462</v>
+        <v>44334</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -10451,7 +10451,7 @@
       </c>
       <c r="C31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44622</v>
+        <v>44516</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -10466,7 +10466,7 @@
       </c>
       <c r="C32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45049</v>
+        <v>44598</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -10481,7 +10481,7 @@
       </c>
       <c r="C33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44734</v>
+        <v>44284</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -10496,7 +10496,7 @@
       </c>
       <c r="C34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45091</v>
+        <v>44498</v>
       </c>
       <c r="D34">
         <v>2</v>
@@ -10511,7 +10511,7 @@
       </c>
       <c r="C35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44795</v>
+        <v>45130</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -10526,7 +10526,7 @@
       </c>
       <c r="C36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45179</v>
+        <v>44243</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -10541,7 +10541,7 @@
       </c>
       <c r="C37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44862</v>
+        <v>44610</v>
       </c>
       <c r="D37">
         <v>1</v>
@@ -10556,7 +10556,7 @@
       </c>
       <c r="C38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44234</v>
+        <v>44216</v>
       </c>
       <c r="D38">
         <v>3</v>
@@ -10571,7 +10571,7 @@
       </c>
       <c r="C39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44912</v>
+        <v>45099</v>
       </c>
       <c r="D39">
         <v>3</v>
@@ -10586,7 +10586,7 @@
       </c>
       <c r="C40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44354</v>
+        <v>44497</v>
       </c>
       <c r="D40">
         <v>1</v>
@@ -10601,7 +10601,7 @@
       </c>
       <c r="C41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44726</v>
+        <v>44776</v>
       </c>
       <c r="D41">
         <v>1</v>
@@ -10616,7 +10616,7 @@
       </c>
       <c r="C42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44397</v>
+        <v>44671</v>
       </c>
       <c r="D42">
         <f t="shared" ref="D42:D84" ca="1" si="1">RANDBETWEEN(0, 4)</f>
@@ -10632,11 +10632,11 @@
       </c>
       <c r="C43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44608</v>
+        <v>44506</v>
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -10648,11 +10648,11 @@
       </c>
       <c r="C44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45159</v>
+        <v>44467</v>
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -10664,11 +10664,11 @@
       </c>
       <c r="C45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44558</v>
+        <v>44513</v>
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -10680,11 +10680,11 @@
       </c>
       <c r="C46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44335</v>
+        <v>44875</v>
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -10696,11 +10696,11 @@
       </c>
       <c r="C47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44546</v>
+        <v>44864</v>
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -10712,7 +10712,7 @@
       </c>
       <c r="C48" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44254</v>
+        <v>44512</v>
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="1"/>
@@ -10728,11 +10728,11 @@
       </c>
       <c r="C49" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44682</v>
+        <v>44337</v>
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -10744,11 +10744,11 @@
       </c>
       <c r="C50" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44506</v>
+        <v>44496</v>
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -10760,11 +10760,11 @@
       </c>
       <c r="C51" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44987</v>
+        <v>45198</v>
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -10776,11 +10776,11 @@
       </c>
       <c r="C52" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>45179</v>
+        <v>44554</v>
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -10792,11 +10792,11 @@
       </c>
       <c r="C53" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44201</v>
+        <v>44268</v>
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -10808,11 +10808,11 @@
       </c>
       <c r="C54" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44340</v>
+        <v>45131</v>
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -10824,7 +10824,7 @@
       </c>
       <c r="C55" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>44912</v>
+        <v>45157</v>
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="1"/>
@@ -10840,11 +10840,11 @@
       </c>
       <c r="C56" s="1">
         <f t="shared" ref="C56:C84" ca="1" si="2">RANDBETWEEN(DATE(2021,1,1),DATE(2023,12,31))</f>
-        <v>44424</v>
+        <v>44544</v>
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -10856,11 +10856,11 @@
       </c>
       <c r="C57" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45264</v>
+        <v>45245</v>
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -10872,11 +10872,11 @@
       </c>
       <c r="C58" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45177</v>
+        <v>44566</v>
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -10888,11 +10888,11 @@
       </c>
       <c r="C59" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45232</v>
+        <v>44885</v>
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -10904,11 +10904,11 @@
       </c>
       <c r="C60" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44813</v>
+        <v>44454</v>
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -10920,11 +10920,11 @@
       </c>
       <c r="C61" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45150</v>
+        <v>44548</v>
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -10936,11 +10936,11 @@
       </c>
       <c r="C62" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44595</v>
+        <v>44737</v>
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -10952,11 +10952,11 @@
       </c>
       <c r="C63" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44622</v>
+        <v>45144</v>
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -10968,11 +10968,11 @@
       </c>
       <c r="C64" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45127</v>
+        <v>44409</v>
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -10984,7 +10984,7 @@
       </c>
       <c r="C65" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44853</v>
+        <v>44944</v>
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="1"/>
@@ -11000,7 +11000,7 @@
       </c>
       <c r="C66" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44813</v>
+        <v>44535</v>
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="1"/>
@@ -11016,11 +11016,11 @@
       </c>
       <c r="C67" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44472</v>
+        <v>44648</v>
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -11032,11 +11032,11 @@
       </c>
       <c r="C68" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44400</v>
+        <v>44782</v>
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -11048,11 +11048,11 @@
       </c>
       <c r="C69" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45205</v>
+        <v>45194</v>
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -11064,7 +11064,7 @@
       </c>
       <c r="C70" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44768</v>
+        <v>44323</v>
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="1"/>
@@ -11080,7 +11080,7 @@
       </c>
       <c r="C71" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44485</v>
+        <v>45062</v>
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="1"/>
@@ -11096,11 +11096,11 @@
       </c>
       <c r="C72" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44664</v>
+        <v>44778</v>
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -11112,11 +11112,11 @@
       </c>
       <c r="C73" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44278</v>
+        <v>44897</v>
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -11128,11 +11128,11 @@
       </c>
       <c r="C74" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44472</v>
+        <v>45044</v>
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -11144,11 +11144,11 @@
       </c>
       <c r="C75" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44284</v>
+        <v>44346</v>
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -11160,11 +11160,11 @@
       </c>
       <c r="C76" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44522</v>
+        <v>44863</v>
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -11176,11 +11176,11 @@
       </c>
       <c r="C77" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44862</v>
+        <v>45061</v>
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -11192,7 +11192,7 @@
       </c>
       <c r="C78" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44742</v>
+        <v>44248</v>
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="1"/>
@@ -11208,11 +11208,11 @@
       </c>
       <c r="C79" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44907</v>
+        <v>44874</v>
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -11224,11 +11224,11 @@
       </c>
       <c r="C80" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44201</v>
+        <v>45201</v>
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -11240,11 +11240,11 @@
       </c>
       <c r="C81" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45121</v>
+        <v>44640</v>
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -11256,11 +11256,11 @@
       </c>
       <c r="C82" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44236</v>
+        <v>45250</v>
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -11272,11 +11272,11 @@
       </c>
       <c r="C83" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>45228</v>
+        <v>44744</v>
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -11288,7 +11288,7 @@
       </c>
       <c r="C84" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>44782</v>
+        <v>44956</v>
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="1"/>

</xml_diff>